<commit_message>
Wersja ze srody - sprzed feedbacku od lekarzy.
git-svn-id: https://localhost:8443/svn/bdr@996 5173494c-6dae-45e1-bfb1-e08744c75a4d
</commit_message>
<xml_diff>
--- a/TPP/dokumenty/TPP_atrybuty1.xlsx
+++ b/TPP/dokumenty/TPP_atrybuty1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="255">
   <si>
     <t>Nazwa atrybutu</t>
   </si>
@@ -778,13 +778,16 @@
   </si>
   <si>
     <t>BadanieWechu</t>
+  </si>
+  <si>
+    <t>wersja 0.4 (2013-07-10)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1207,7 +1210,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1288,9 +1291,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1328,7 +1331,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1362,7 +1365,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1397,10 +1399,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1573,14 +1574,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D192"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A168" sqref="A168"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="52.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
@@ -1589,7 +1588,12 @@
     <col min="5" max="16384" width="9.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
@@ -1603,7 +1607,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="55" t="s">
         <v>4</v>
       </c>
@@ -1613,7 +1617,7 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1623,7 +1627,7 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1633,7 +1637,7 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1645,7 +1649,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1657,7 +1661,7 @@
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
@@ -1669,7 +1673,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1681,7 +1685,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
@@ -1693,7 +1697,7 @@
       </c>
       <c r="D10" s="13"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" thickTop="1">
       <c r="A11" s="56" t="s">
         <v>10</v>
       </c>
@@ -1705,7 +1709,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1715,7 +1719,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
@@ -1727,7 +1731,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
@@ -1737,7 +1741,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1747,7 +1751,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1757,7 +1761,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -1768,7 +1772,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -1780,7 +1784,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
@@ -1790,7 +1794,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1802,7 +1806,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>37</v>
       </c>
@@ -1814,7 +1818,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1824,7 +1828,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1836,7 +1840,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
@@ -1846,7 +1850,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
@@ -1856,7 +1860,7 @@
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
@@ -1868,7 +1872,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
@@ -1880,7 +1884,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
@@ -1890,7 +1894,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>237</v>
       </c>
@@ -1900,7 +1904,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>48</v>
       </c>
@@ -1912,7 +1916,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4">
       <c r="A31" s="2" t="s">
         <v>238</v>
       </c>
@@ -1922,7 +1926,7 @@
       <c r="C31" s="4"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
@@ -1934,7 +1938,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
@@ -1944,7 +1948,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>52</v>
       </c>
@@ -1956,7 +1960,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="2" t="s">
         <v>53</v>
       </c>
@@ -1966,7 +1970,7 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>54</v>
       </c>
@@ -1978,7 +1982,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>55</v>
       </c>
@@ -1988,7 +1992,7 @@
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>56</v>
       </c>
@@ -2000,7 +2004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
         <v>57</v>
       </c>
@@ -2010,7 +2014,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>58</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>59</v>
       </c>
@@ -2032,7 +2036,7 @@
       <c r="C41" s="2"/>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>60</v>
       </c>
@@ -2044,7 +2048,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
         <v>63</v>
       </c>
@@ -2056,7 +2060,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>65</v>
       </c>
@@ -2068,7 +2072,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>67</v>
       </c>
@@ -2080,7 +2084,7 @@
       </c>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>69</v>
       </c>
@@ -2090,7 +2094,7 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
         <v>70</v>
       </c>
@@ -2102,7 +2106,7 @@
       </c>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>72</v>
       </c>
@@ -2112,7 +2116,7 @@
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>73</v>
       </c>
@@ -2124,7 +2128,7 @@
       </c>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>75</v>
       </c>
@@ -2136,7 +2140,7 @@
       </c>
       <c r="D50" s="2"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="2" t="s">
         <v>77</v>
       </c>
@@ -2146,7 +2150,7 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>78</v>
       </c>
@@ -2156,7 +2160,7 @@
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>79</v>
       </c>
@@ -2170,7 +2174,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1">
       <c r="A54" s="13" t="s">
         <v>82</v>
       </c>
@@ -2182,7 +2186,7 @@
       </c>
       <c r="D54" s="13"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="15.75" thickTop="1">
       <c r="A55" s="6" t="s">
         <v>85</v>
       </c>
@@ -2194,7 +2198,7 @@
       </c>
       <c r="D55" s="53"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>87</v>
       </c>
@@ -2206,7 +2210,7 @@
       </c>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>88</v>
       </c>
@@ -2218,7 +2222,7 @@
       </c>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>89</v>
       </c>
@@ -2230,7 +2234,7 @@
       </c>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
         <v>90</v>
       </c>
@@ -2242,7 +2246,7 @@
       </c>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>91</v>
       </c>
@@ -2254,7 +2258,7 @@
       </c>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>92</v>
       </c>
@@ -2266,7 +2270,7 @@
       </c>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>93</v>
       </c>
@@ -2278,7 +2282,7 @@
       </c>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
         <v>94</v>
       </c>
@@ -2290,7 +2294,7 @@
       </c>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>95</v>
       </c>
@@ -2302,7 +2306,7 @@
       </c>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>96</v>
       </c>
@@ -2314,7 +2318,7 @@
       </c>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>97</v>
       </c>
@@ -2326,7 +2330,7 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
         <v>98</v>
       </c>
@@ -2338,7 +2342,7 @@
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>99</v>
       </c>
@@ -2350,7 +2354,7 @@
       </c>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>100</v>
       </c>
@@ -2362,7 +2366,7 @@
       </c>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
         <v>101</v>
       </c>
@@ -2374,7 +2378,7 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4">
       <c r="A71" s="2" t="s">
         <v>102</v>
       </c>
@@ -2386,7 +2390,7 @@
       </c>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>103</v>
       </c>
@@ -2398,7 +2402,7 @@
       </c>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
         <v>104</v>
       </c>
@@ -2410,7 +2414,7 @@
       </c>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
         <v>105</v>
       </c>
@@ -2422,7 +2426,7 @@
       </c>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
         <v>106</v>
       </c>
@@ -2434,7 +2438,7 @@
       </c>
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
         <v>107</v>
       </c>
@@ -2446,7 +2450,7 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4">
       <c r="A77" s="2" t="s">
         <v>108</v>
       </c>
@@ -2458,7 +2462,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
         <v>109</v>
       </c>
@@ -2470,7 +2474,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4">
       <c r="A79" s="2" t="s">
         <v>110</v>
       </c>
@@ -2482,7 +2486,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
         <v>111</v>
       </c>
@@ -2494,7 +2498,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" ht="15.75" thickBot="1">
       <c r="A81" s="13" t="s">
         <v>112</v>
       </c>
@@ -2506,7 +2510,7 @@
       </c>
       <c r="D81" s="13"/>
     </row>
-    <row r="82" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15.75" thickTop="1">
       <c r="A82" s="6" t="s">
         <v>113</v>
       </c>
@@ -2518,7 +2522,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4">
       <c r="A83" s="2" t="s">
         <v>115</v>
       </c>
@@ -2528,7 +2532,7 @@
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
         <v>116</v>
       </c>
@@ -2538,7 +2542,7 @@
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>117</v>
       </c>
@@ -2550,7 +2554,7 @@
       </c>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
         <v>119</v>
       </c>
@@ -2560,7 +2564,7 @@
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
         <v>120</v>
       </c>
@@ -2572,7 +2576,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
         <v>122</v>
       </c>
@@ -2582,7 +2586,7 @@
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4">
       <c r="A89" s="2" t="s">
         <v>123</v>
       </c>
@@ -2594,7 +2598,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
         <v>125</v>
       </c>
@@ -2606,7 +2610,7 @@
       </c>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
         <v>127</v>
       </c>
@@ -2616,7 +2620,7 @@
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
         <v>253</v>
       </c>
@@ -2626,7 +2630,7 @@
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
         <v>128</v>
       </c>
@@ -2638,7 +2642,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
         <v>239</v>
       </c>
@@ -2648,7 +2652,7 @@
       <c r="C94" s="4"/>
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4">
       <c r="A95" s="2" t="s">
         <v>130</v>
       </c>
@@ -2660,7 +2664,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4">
       <c r="A96" s="5" t="s">
         <v>132</v>
       </c>
@@ -2672,7 +2676,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4">
       <c r="A97" s="21" t="s">
         <v>247</v>
       </c>
@@ -2686,7 +2690,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4">
       <c r="A98" s="23" t="s">
         <v>135</v>
       </c>
@@ -2696,7 +2700,7 @@
       <c r="C98" s="24"/>
       <c r="D98" s="24"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4">
       <c r="A99" s="24" t="s">
         <v>136</v>
       </c>
@@ -2706,7 +2710,7 @@
       <c r="C99" s="24"/>
       <c r="D99" s="24"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4">
       <c r="A100" s="24" t="s">
         <v>137</v>
       </c>
@@ -2716,7 +2720,7 @@
       <c r="C100" s="24"/>
       <c r="D100" s="24"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4">
       <c r="A101" s="24" t="s">
         <v>138</v>
       </c>
@@ -2726,7 +2730,7 @@
       <c r="C101" s="24"/>
       <c r="D101" s="24"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4">
       <c r="A102" s="24" t="s">
         <v>139</v>
       </c>
@@ -2736,7 +2740,7 @@
       <c r="C102" s="24"/>
       <c r="D102" s="24"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4">
       <c r="A103" s="24" t="s">
         <v>140</v>
       </c>
@@ -2746,7 +2750,7 @@
       <c r="C103" s="24"/>
       <c r="D103" s="24"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4">
       <c r="A104" s="24" t="s">
         <v>141</v>
       </c>
@@ -2756,7 +2760,7 @@
       <c r="C104" s="24"/>
       <c r="D104" s="24"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4">
       <c r="A105" s="24" t="s">
         <v>142</v>
       </c>
@@ -2766,7 +2770,7 @@
       <c r="C105" s="24"/>
       <c r="D105" s="24"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4">
       <c r="A106" s="24" t="s">
         <v>143</v>
       </c>
@@ -2776,7 +2780,7 @@
       <c r="C106" s="24"/>
       <c r="D106" s="24"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4">
       <c r="A107" s="24" t="s">
         <v>144</v>
       </c>
@@ -2786,7 +2790,7 @@
       <c r="C107" s="24"/>
       <c r="D107" s="24"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4">
       <c r="A108" s="24" t="s">
         <v>145</v>
       </c>
@@ -2796,7 +2800,7 @@
       <c r="C108" s="24"/>
       <c r="D108" s="24"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4">
       <c r="A109" s="24" t="s">
         <v>146</v>
       </c>
@@ -2806,7 +2810,7 @@
       <c r="C109" s="24"/>
       <c r="D109" s="24"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4">
       <c r="A110" s="24" t="s">
         <v>147</v>
       </c>
@@ -2816,7 +2820,7 @@
       <c r="C110" s="24"/>
       <c r="D110" s="24"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4">
       <c r="A111" s="24" t="s">
         <v>148</v>
       </c>
@@ -2826,7 +2830,7 @@
       <c r="C111" s="24"/>
       <c r="D111" s="24"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4">
       <c r="A112" s="24" t="s">
         <v>149</v>
       </c>
@@ -2836,7 +2840,7 @@
       <c r="C112" s="24"/>
       <c r="D112" s="24"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4">
       <c r="A113" s="24" t="s">
         <v>150</v>
       </c>
@@ -2846,7 +2850,7 @@
       <c r="C113" s="24"/>
       <c r="D113" s="24"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4">
       <c r="A114" s="24" t="s">
         <v>151</v>
       </c>
@@ -2856,7 +2860,7 @@
       <c r="C114" s="24"/>
       <c r="D114" s="24"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4">
       <c r="A115" s="24" t="s">
         <v>152</v>
       </c>
@@ -2866,7 +2870,7 @@
       <c r="C115" s="24"/>
       <c r="D115" s="24"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4">
       <c r="A116" s="24" t="s">
         <v>153</v>
       </c>
@@ -2876,7 +2880,7 @@
       <c r="C116" s="24"/>
       <c r="D116" s="24"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4">
       <c r="A117" s="24" t="s">
         <v>154</v>
       </c>
@@ -2886,7 +2890,7 @@
       <c r="C117" s="24"/>
       <c r="D117" s="24"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4">
       <c r="A118" s="24" t="s">
         <v>155</v>
       </c>
@@ -2896,7 +2900,7 @@
       <c r="C118" s="24"/>
       <c r="D118" s="24"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4">
       <c r="A119" s="24" t="s">
         <v>156</v>
       </c>
@@ -2906,7 +2910,7 @@
       <c r="C119" s="24"/>
       <c r="D119" s="24"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4">
       <c r="A120" s="24" t="s">
         <v>157</v>
       </c>
@@ -2916,7 +2920,7 @@
       <c r="C120" s="24"/>
       <c r="D120" s="24"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4">
       <c r="A121" s="24" t="s">
         <v>158</v>
       </c>
@@ -2926,7 +2930,7 @@
       <c r="C121" s="24"/>
       <c r="D121" s="24"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4">
       <c r="A122" s="24" t="s">
         <v>159</v>
       </c>
@@ -2936,7 +2940,7 @@
       <c r="C122" s="24"/>
       <c r="D122" s="24"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4">
       <c r="A123" s="24" t="s">
         <v>160</v>
       </c>
@@ -2946,7 +2950,7 @@
       <c r="C123" s="24"/>
       <c r="D123" s="24"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4">
       <c r="A124" s="24" t="s">
         <v>161</v>
       </c>
@@ -2956,7 +2960,7 @@
       <c r="C124" s="24"/>
       <c r="D124" s="24"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4">
       <c r="A125" s="24" t="s">
         <v>162</v>
       </c>
@@ -2966,7 +2970,7 @@
       <c r="C125" s="24"/>
       <c r="D125" s="24"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4">
       <c r="A126" s="24" t="s">
         <v>163</v>
       </c>
@@ -2976,7 +2980,7 @@
       <c r="C126" s="24"/>
       <c r="D126" s="24"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4">
       <c r="A127" s="24" t="s">
         <v>164</v>
       </c>
@@ -2986,7 +2990,7 @@
       <c r="C127" s="24"/>
       <c r="D127" s="24"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4">
       <c r="A128" s="24" t="s">
         <v>165</v>
       </c>
@@ -2996,7 +3000,7 @@
       <c r="C128" s="24"/>
       <c r="D128" s="24"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4">
       <c r="A129" s="24" t="s">
         <v>166</v>
       </c>
@@ -3006,7 +3010,7 @@
       <c r="C129" s="24"/>
       <c r="D129" s="24"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4">
       <c r="A130" s="43" t="s">
         <v>167</v>
       </c>
@@ -3016,7 +3020,7 @@
       <c r="C130" s="43"/>
       <c r="D130" s="43"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4">
       <c r="A131" s="6" t="s">
         <v>168</v>
       </c>
@@ -3026,7 +3030,7 @@
       <c r="C131" s="6"/>
       <c r="D131" s="6"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4">
       <c r="A132" s="2" t="s">
         <v>169</v>
       </c>
@@ -3036,7 +3040,7 @@
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4">
       <c r="A133" s="2" t="s">
         <v>170</v>
       </c>
@@ -3046,7 +3050,7 @@
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4">
       <c r="A134" s="7" t="s">
         <v>171</v>
       </c>
@@ -3056,7 +3060,7 @@
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4">
       <c r="A135" s="6" t="s">
         <v>172</v>
       </c>
@@ -3068,7 +3072,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4">
       <c r="A136" s="2" t="s">
         <v>174</v>
       </c>
@@ -3080,7 +3084,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4">
       <c r="A137" s="2" t="s">
         <v>176</v>
       </c>
@@ -3090,7 +3094,7 @@
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4">
       <c r="A138" s="2" t="s">
         <v>177</v>
       </c>
@@ -3100,7 +3104,7 @@
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4">
       <c r="A139" s="2" t="s">
         <v>178</v>
       </c>
@@ -3110,7 +3114,7 @@
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4">
       <c r="A140" s="2" t="s">
         <v>179</v>
       </c>
@@ -3120,7 +3124,7 @@
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4">
       <c r="A141" s="2" t="s">
         <v>180</v>
       </c>
@@ -3130,7 +3134,7 @@
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4">
       <c r="A142" s="2" t="s">
         <v>181</v>
       </c>
@@ -3140,7 +3144,7 @@
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4">
       <c r="A143" s="2" t="s">
         <v>182</v>
       </c>
@@ -3150,7 +3154,7 @@
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4">
       <c r="A144" s="2" t="s">
         <v>183</v>
       </c>
@@ -3160,7 +3164,7 @@
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4">
       <c r="A145" s="2" t="s">
         <v>184</v>
       </c>
@@ -3170,7 +3174,7 @@
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4">
       <c r="A146" s="2" t="s">
         <v>185</v>
       </c>
@@ -3180,7 +3184,7 @@
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="15.75" thickBot="1">
       <c r="A147" s="13" t="s">
         <v>186</v>
       </c>
@@ -3192,7 +3196,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="148" spans="1:4" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="16.5" customHeight="1" thickTop="1">
       <c r="A148" s="21" t="s">
         <v>242</v>
       </c>
@@ -3206,7 +3210,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4">
       <c r="A149" s="30" t="s">
         <v>247</v>
       </c>
@@ -3218,7 +3222,7 @@
       </c>
       <c r="D149" s="31"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4">
       <c r="A150" s="32" t="s">
         <v>135</v>
       </c>
@@ -3230,7 +3234,7 @@
       </c>
       <c r="D150" s="33"/>
     </row>
-    <row r="151" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" s="14" customFormat="1">
       <c r="A151" s="34" t="s">
         <v>241</v>
       </c>
@@ -3240,7 +3244,7 @@
       <c r="C151" s="35"/>
       <c r="D151" s="36"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4">
       <c r="A152" s="22" t="s">
         <v>188</v>
       </c>
@@ -3250,7 +3254,7 @@
       <c r="C152" s="29"/>
       <c r="D152" s="22"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4">
       <c r="A153" s="24" t="s">
         <v>189</v>
       </c>
@@ -3260,7 +3264,7 @@
       <c r="C153" s="37"/>
       <c r="D153" s="24"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4">
       <c r="A154" s="24" t="s">
         <v>190</v>
       </c>
@@ -3270,7 +3274,7 @@
       <c r="C154" s="24"/>
       <c r="D154" s="24"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4">
       <c r="A155" s="24" t="s">
         <v>192</v>
       </c>
@@ -3280,7 +3284,7 @@
       <c r="C155" s="37"/>
       <c r="D155" s="24"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4">
       <c r="A156" s="24" t="s">
         <v>193</v>
       </c>
@@ -3290,7 +3294,7 @@
       <c r="C156" s="24"/>
       <c r="D156" s="24"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4">
       <c r="A157" s="38" t="s">
         <v>194</v>
       </c>
@@ -3300,7 +3304,7 @@
       <c r="C157" s="38"/>
       <c r="D157" s="38"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4">
       <c r="A158" s="34" t="s">
         <v>195</v>
       </c>
@@ -3310,7 +3314,7 @@
       <c r="C158" s="34"/>
       <c r="D158" s="34"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4">
       <c r="A159" s="39" t="s">
         <v>196</v>
       </c>
@@ -3322,7 +3326,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4">
       <c r="A160" s="39" t="s">
         <v>199</v>
       </c>
@@ -3332,7 +3336,7 @@
       <c r="C160" s="39"/>
       <c r="D160" s="42"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4">
       <c r="A161" s="39" t="s">
         <v>200</v>
       </c>
@@ -3342,7 +3346,7 @@
       <c r="C161" s="39"/>
       <c r="D161" s="42"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4">
       <c r="A162" s="39" t="s">
         <v>201</v>
       </c>
@@ -3354,7 +3358,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4">
       <c r="A163" s="39" t="s">
         <v>203</v>
       </c>
@@ -3364,7 +3368,7 @@
       <c r="C163" s="39"/>
       <c r="D163" s="42"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4">
       <c r="A164" s="22" t="s">
         <v>204</v>
       </c>
@@ -3376,7 +3380,7 @@
       </c>
       <c r="D164" s="24"/>
     </row>
-    <row r="165" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="15.75" thickBot="1">
       <c r="A165" s="26" t="s">
         <v>206</v>
       </c>
@@ -3388,7 +3392,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" ht="15.75" thickTop="1">
       <c r="A166" s="6" t="s">
         <v>208</v>
       </c>
@@ -3398,7 +3402,7 @@
       <c r="C166" s="6"/>
       <c r="D166" s="6"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4">
       <c r="A167" s="2" t="s">
         <v>209</v>
       </c>
@@ -3408,7 +3412,7 @@
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4">
       <c r="A168" s="2" t="s">
         <v>210</v>
       </c>
@@ -3418,7 +3422,7 @@
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4">
       <c r="A169" s="2" t="s">
         <v>211</v>
       </c>
@@ -3428,7 +3432,7 @@
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4">
       <c r="A170" s="2" t="s">
         <v>212</v>
       </c>
@@ -3438,7 +3442,7 @@
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4">
       <c r="A171" s="2" t="s">
         <v>213</v>
       </c>
@@ -3450,7 +3454,7 @@
       </c>
       <c r="D171" s="2"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4">
       <c r="A172" s="2" t="s">
         <v>215</v>
       </c>
@@ -3462,7 +3466,7 @@
       </c>
       <c r="D172" s="2"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4">
       <c r="A173" s="2" t="s">
         <v>217</v>
       </c>
@@ -3472,7 +3476,7 @@
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4">
       <c r="A174" s="2" t="s">
         <v>218</v>
       </c>
@@ -3482,7 +3486,7 @@
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4">
       <c r="A175" s="2" t="s">
         <v>219</v>
       </c>
@@ -3492,7 +3496,7 @@
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
     </row>
-    <row r="176" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="15.75" thickBot="1">
       <c r="A176" s="13" t="s">
         <v>220</v>
       </c>
@@ -3502,7 +3506,7 @@
       <c r="C176" s="13"/>
       <c r="D176" s="13"/>
     </row>
-    <row r="177" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" ht="15.75" thickTop="1">
       <c r="A177" s="21" t="s">
         <v>247</v>
       </c>
@@ -3514,7 +3518,7 @@
       </c>
       <c r="D177" s="22"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4">
       <c r="A178" s="23" t="s">
         <v>135</v>
       </c>
@@ -3524,7 +3528,7 @@
       <c r="C178" s="24"/>
       <c r="D178" s="24"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4">
       <c r="A179" s="24" t="s">
         <v>221</v>
       </c>
@@ -3534,7 +3538,7 @@
       <c r="C179" s="25"/>
       <c r="D179" s="24"/>
     </row>
-    <row r="180" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" ht="15.75" thickBot="1">
       <c r="A180" s="26" t="s">
         <v>246</v>
       </c>
@@ -3544,13 +3548,13 @@
       <c r="C180" s="27"/>
       <c r="D180" s="26"/>
     </row>
-    <row r="181" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" ht="15.75" thickTop="1">
       <c r="A181" s="6"/>
       <c r="B181" s="6"/>
       <c r="C181" s="6"/>
       <c r="D181" s="6"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4">
       <c r="A183" s="19"/>
       <c r="B183" s="19"/>
       <c r="C183" s="19" t="s">
@@ -3558,7 +3562,7 @@
       </c>
       <c r="D183" s="19"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4">
       <c r="A184" s="20" t="s">
         <v>223</v>
       </c>
@@ -3572,7 +3576,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4">
       <c r="A185" s="20" t="s">
         <v>226</v>
       </c>
@@ -3584,7 +3588,7 @@
       </c>
       <c r="D185" s="20"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4">
       <c r="A186" s="20" t="s">
         <v>227</v>
       </c>
@@ -3592,13 +3596,13 @@
       <c r="C186" s="20"/>
       <c r="D186" s="20"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="C187" s="8"/>
       <c r="D187" s="8"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4">
       <c r="A188" s="8"/>
       <c r="B188" s="8" t="s">
         <v>228</v>
@@ -3606,7 +3610,7 @@
       <c r="C188" s="8"/>
       <c r="D188" s="8"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4">
       <c r="C189" s="11" t="s">
         <v>229</v>
       </c>
@@ -3614,7 +3618,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4">
       <c r="C190" s="11" t="s">
         <v>230</v>
       </c>
@@ -3622,7 +3626,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4">
       <c r="C191" s="11" t="s">
         <v>231</v>
       </c>
@@ -3630,7 +3634,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4">
       <c r="C192" s="11" t="s">
         <v>232</v>
       </c>
@@ -3648,20 +3652,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:FV28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="9.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:178" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:178" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:178" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:178" ht="15.75" thickBot="1">
       <c r="A2" s="8"/>
       <c r="B2" s="44" t="s">
         <v>248</v>
@@ -3742,7 +3746,7 @@
       <c r="FU2" s="45"/>
       <c r="FV2" s="46"/>
     </row>
-    <row r="3" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:178">
       <c r="A3" s="8"/>
       <c r="B3" s="12" t="s">
         <v>4</v>
@@ -4274,7 +4278,7 @@
       </c>
       <c r="FV3" s="12"/>
     </row>
-    <row r="4" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:178">
       <c r="A4" s="8"/>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -4454,7 +4458,7 @@
       <c r="FU4" s="39"/>
       <c r="FV4" s="18"/>
     </row>
-    <row r="5" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:178">
       <c r="A5" s="8"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
@@ -4634,7 +4638,7 @@
       <c r="FU5" s="39"/>
       <c r="FV5" s="18"/>
     </row>
-    <row r="6" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:178">
       <c r="A6" s="8"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -4814,7 +4818,7 @@
       <c r="FU6" s="39"/>
       <c r="FV6" s="18"/>
     </row>
-    <row r="7" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:178">
       <c r="A7" s="8"/>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -4994,7 +4998,7 @@
       <c r="FU7" s="39"/>
       <c r="FV7" s="18"/>
     </row>
-    <row r="8" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:178">
       <c r="A8" s="8"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -5174,7 +5178,7 @@
       <c r="FU8" s="39"/>
       <c r="FV8" s="18"/>
     </row>
-    <row r="9" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:178">
       <c r="A9" s="8"/>
       <c r="B9" s="18"/>
       <c r="C9" s="18"/>
@@ -5354,7 +5358,7 @@
       <c r="FU9" s="39"/>
       <c r="FV9" s="18"/>
     </row>
-    <row r="10" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:178">
       <c r="A10" s="8"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
@@ -5534,7 +5538,7 @@
       <c r="FU10" s="39"/>
       <c r="FV10" s="18"/>
     </row>
-    <row r="11" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:178">
       <c r="A11" s="8"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -5714,7 +5718,7 @@
       <c r="FU11" s="39"/>
       <c r="FV11" s="18"/>
     </row>
-    <row r="12" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:178">
       <c r="A12" s="8"/>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -5894,7 +5898,7 @@
       <c r="FU12" s="39"/>
       <c r="FV12" s="18"/>
     </row>
-    <row r="13" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:178">
       <c r="A13" s="8"/>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -6074,7 +6078,7 @@
       <c r="FU13" s="39"/>
       <c r="FV13" s="18"/>
     </row>
-    <row r="14" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:178">
       <c r="A14" s="8"/>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -6254,7 +6258,7 @@
       <c r="FU14" s="39"/>
       <c r="FV14" s="18"/>
     </row>
-    <row r="15" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:178">
       <c r="A15" s="8"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -6434,7 +6438,7 @@
       <c r="FU15" s="39"/>
       <c r="FV15" s="18"/>
     </row>
-    <row r="16" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:178">
       <c r="A16" s="8"/>
       <c r="B16" s="18"/>
       <c r="C16" s="18"/>
@@ -6614,7 +6618,7 @@
       <c r="FU16" s="39"/>
       <c r="FV16" s="18"/>
     </row>
-    <row r="17" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:178">
       <c r="A17" s="8"/>
       <c r="B17" s="18"/>
       <c r="C17" s="18"/>
@@ -6794,7 +6798,7 @@
       <c r="FU17" s="39"/>
       <c r="FV17" s="18"/>
     </row>
-    <row r="18" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:178">
       <c r="A18" s="8"/>
       <c r="B18" s="18"/>
       <c r="C18" s="18"/>
@@ -6974,7 +6978,7 @@
       <c r="FU18" s="39"/>
       <c r="FV18" s="18"/>
     </row>
-    <row r="19" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:178">
       <c r="A19" s="8"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -7154,7 +7158,7 @@
       <c r="FU19" s="39"/>
       <c r="FV19" s="18"/>
     </row>
-    <row r="20" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:178">
       <c r="A20" s="8"/>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -7334,7 +7338,7 @@
       <c r="FU20" s="39"/>
       <c r="FV20" s="18"/>
     </row>
-    <row r="21" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:178">
       <c r="A21" s="8"/>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -7514,7 +7518,7 @@
       <c r="FU21" s="39"/>
       <c r="FV21" s="18"/>
     </row>
-    <row r="22" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:178">
       <c r="A22" s="8"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -7694,7 +7698,7 @@
       <c r="FU22" s="39"/>
       <c r="FV22" s="18"/>
     </row>
-    <row r="23" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:178">
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
@@ -7873,7 +7877,7 @@
       <c r="FU23" s="39"/>
       <c r="FV23" s="18"/>
     </row>
-    <row r="24" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:178">
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -8052,7 +8056,7 @@
       <c r="FU24" s="39"/>
       <c r="FV24" s="18"/>
     </row>
-    <row r="25" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:178">
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -8231,7 +8235,7 @@
       <c r="FU25" s="39"/>
       <c r="FV25" s="18"/>
     </row>
-    <row r="26" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:178">
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
@@ -8410,7 +8414,7 @@
       <c r="FU26" s="39"/>
       <c r="FV26" s="18"/>
     </row>
-    <row r="27" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:178">
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
@@ -8589,7 +8593,7 @@
       <c r="FU27" s="39"/>
       <c r="FV27" s="18"/>
     </row>
-    <row r="28" spans="1:178" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:178">
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
@@ -8778,12 +8782,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="9.42578125" style="1"/>
   </cols>

</xml_diff>

<commit_message>
Poprawki przy implementacji części niewariantowej danych badania.
git-svn-id: https://localhost:8443/svn/bdr@1013 5173494c-6dae-45e1-bfb1-e08744c75a4d
</commit_message>
<xml_diff>
--- a/TPP/dokumenty/TPP_atrybuty1.xlsx
+++ b/TPP/dokumenty/TPP_atrybuty1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="274">
   <si>
     <t>Nazwa atrybutu</t>
   </si>
@@ -510,12 +510,6 @@
     <t>0-30</t>
   </si>
   <si>
-    <t>WAIS-R_Wiadomosci</t>
-  </si>
-  <si>
-    <t>WAIS-R_PowtarzanieCyfr</t>
-  </si>
-  <si>
     <t>SkalaDepresjiBecka</t>
   </si>
   <si>
@@ -625,9 +619,6 @@
   </si>
   <si>
     <t>USGWynik</t>
-  </si>
-  <si>
-    <t>0=brak okna; 1=brak hyperechogeniczności; 2=hyperechgeniczność</t>
   </si>
   <si>
     <t>Genetyka</t>
@@ -844,6 +835,21 @@
   </si>
   <si>
     <t>&lt;wybrać nazwę5&gt;  (cz. H)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = @</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>WAIS_R_Wiadomosci</t>
+  </si>
+  <si>
+    <t>WAIS_R_PowtarzanieCyfr</t>
+  </si>
+  <si>
+    <t>0=brak okna; 1=brak hyperechogeniczności; 2=hyperechogeniczność</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1358,6 +1364,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -1730,8 +1737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,7 +1753,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,7 +1773,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>4</v>
@@ -1811,21 +1818,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="57" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="D7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="44" t="s">
         <v>234</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>235</v>
-      </c>
-      <c r="D7" t="s">
-        <v>252</v>
-      </c>
-      <c r="E7" s="44" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="57" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C8" s="44" t="s">
         <v>9</v>
@@ -1848,10 +1855,10 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
@@ -1863,10 +1870,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1874,17 +1881,17 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="31" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B13" s="76" t="s">
         <v>19</v>
@@ -1896,7 +1903,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1920,7 +1927,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -1951,7 +1958,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1971,7 +1978,7 @@
         <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
@@ -2061,7 +2068,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>106</v>
@@ -2260,10 +2267,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>17</v>
@@ -2285,7 +2292,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>17</v>
@@ -2418,7 +2425,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>56</v>
@@ -2480,13 +2487,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D65" s="60" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E65" s="4"/>
     </row>
@@ -2505,7 +2512,7 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="50"/>
       <c r="B67" s="31" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C67" s="31" t="s">
         <v>9</v>
@@ -2515,7 +2522,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>78</v>
@@ -2843,16 +2850,16 @@
     </row>
     <row r="95" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E95" s="15" t="s">
         <v>123</v>
@@ -2860,14 +2867,14 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" s="16" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C96" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D96" s="17"/>
       <c r="E96" s="17" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
@@ -3192,7 +3199,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B129" s="21" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C129" s="21" t="s">
         <v>10</v>
@@ -3202,34 +3209,34 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B130" s="56" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C130" s="33" t="s">
         <v>9</v>
       </c>
       <c r="D130" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E130" s="20"/>
     </row>
     <row r="131" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="36" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C131" s="21" t="s">
         <v>9</v>
       </c>
       <c r="D131" s="37" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E131" s="22" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="50"/>
       <c r="B132" s="33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C132" s="33" t="s">
         <v>17</v>
@@ -3239,10 +3246,10 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B133" s="54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C133" s="15" t="s">
         <v>17</v>
@@ -3252,7 +3259,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B134" s="17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C134" s="17" t="s">
         <v>17</v>
@@ -3262,27 +3269,27 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B135" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C135" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D135" s="17"/>
       <c r="E135" s="17"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B136" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C136" s="17" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D136" s="23"/>
       <c r="E136" s="17"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B137" s="17" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C137" s="17" t="s">
         <v>17</v>
@@ -3292,10 +3299,10 @@
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B138" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C138" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D138" s="24"/>
       <c r="E138" s="24"/>
@@ -3303,17 +3310,17 @@
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C139" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D139" s="21"/>
       <c r="E139" s="59"/>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B140" s="15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C140" s="15" t="s">
         <v>17</v>
@@ -3324,7 +3331,7 @@
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="50"/>
       <c r="B141" s="32" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C141" s="32" t="s">
         <v>17</v>
@@ -3334,26 +3341,26 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B142" s="39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C142" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D142" s="40"/>
       <c r="E142" s="26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C143" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D143" s="25"/>
       <c r="E143" s="27"/>
@@ -3361,10 +3368,10 @@
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C144" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D144" s="25"/>
       <c r="E144" s="27"/>
@@ -3372,23 +3379,23 @@
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C145" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D145" s="25"/>
       <c r="E145" s="27" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C146" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D146" s="25"/>
       <c r="E146" s="27"/>
@@ -3396,32 +3403,32 @@
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C147" s="15" t="s">
         <v>9</v>
       </c>
       <c r="D147" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E147" s="17"/>
     </row>
     <row r="148" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="52"/>
       <c r="B148" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C148" s="18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D148" s="18"/>
       <c r="E148" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>156</v>
@@ -3465,19 +3472,19 @@
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="50"/>
       <c r="B153" s="63" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C153" s="64" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D153" s="64"/>
       <c r="E153" s="64" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>160</v>
@@ -3504,7 +3511,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
-        <v>164</v>
+        <v>271</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>9</v>
@@ -3514,7 +3521,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
-        <v>165</v>
+        <v>272</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>9</v>
@@ -3524,7 +3531,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B158" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>9</v>
@@ -3534,7 +3541,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B159" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>9</v>
@@ -3544,7 +3551,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B160" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>9</v>
@@ -3554,7 +3561,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B161" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>9</v>
@@ -3564,7 +3571,7 @@
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B162" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>9</v>
@@ -3574,7 +3581,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>9</v>
@@ -3584,7 +3591,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B164" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>9</v>
@@ -3594,7 +3601,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B165" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>9</v>
@@ -3604,7 +3611,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B166" s="31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C166" s="31" t="s">
         <v>9</v>
@@ -3615,20 +3622,20 @@
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="50"/>
       <c r="B167" s="68" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C167" s="64" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D167" s="64"/>
       <c r="E167" s="69"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C168" s="11" t="s">
         <v>17</v>
@@ -3638,7 +3645,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>17</v>
@@ -3648,7 +3655,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B170" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C170" s="6" t="s">
         <v>17</v>
@@ -3658,7 +3665,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B171" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C171" s="6" t="s">
         <v>17</v>
@@ -3668,7 +3675,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B172" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>76</v>
@@ -3678,41 +3685,41 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E173" s="2"/>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B174" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>203</v>
+        <v>273</v>
       </c>
       <c r="E174" s="2"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B175" s="30" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B176" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>17</v>
@@ -3722,7 +3729,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B177" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>76</v>
@@ -3732,7 +3739,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B178" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>17</v>
@@ -3743,7 +3750,7 @@
     <row r="179" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A179" s="65"/>
       <c r="B179" s="42" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C179" s="42" t="s">
         <v>76</v>
@@ -3761,39 +3768,39 @@
       <c r="B182" s="12"/>
       <c r="C182" s="12"/>
       <c r="D182" s="12" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E182" s="12"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B183" s="13" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C183" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D183" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E183" s="13" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B184" s="13" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C184" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D184" s="13" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E184" s="13"/>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B185" s="13" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C185" s="13"/>
       <c r="D185" s="13"/>
@@ -3808,41 +3815,41 @@
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B187" s="5"/>
       <c r="C187" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D187" s="5"/>
       <c r="E187" s="5"/>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D188" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E188" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D189" s="8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E189" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D190" s="8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E190" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D191" s="8" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E191" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -3856,18 +3863,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:FV28"/>
+  <dimension ref="B3:FW31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J5" sqref="J5:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="70"/>
+    <col min="1" max="9" width="9.42578125" style="70"/>
+    <col min="10" max="10" width="50.140625" style="70" customWidth="1"/>
+    <col min="11" max="11" width="65" style="70" customWidth="1"/>
+    <col min="12" max="16384" width="9.42578125" style="70"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:178" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B3" s="71"/>
       <c r="C3" s="71"/>
       <c r="D3" s="71"/>
@@ -3960,9 +3970,9 @@
       <c r="CM3" s="71"/>
       <c r="CN3" s="71"/>
       <c r="CO3" s="71"/>
-      <c r="CP3" s="72"/>
+      <c r="CP3" s="71"/>
       <c r="CQ3" s="72"/>
-      <c r="CR3" s="71"/>
+      <c r="CR3" s="72"/>
       <c r="CS3" s="71"/>
       <c r="CT3" s="71"/>
       <c r="CU3" s="71"/>
@@ -4011,10 +4021,10 @@
       <c r="EL3" s="71"/>
       <c r="EM3" s="71"/>
       <c r="EN3" s="71"/>
-      <c r="EO3" s="72"/>
+      <c r="EO3" s="71"/>
       <c r="EP3" s="72"/>
       <c r="EQ3" s="72"/>
-      <c r="ER3" s="71"/>
+      <c r="ER3" s="72"/>
       <c r="ES3" s="71"/>
       <c r="ET3" s="71"/>
       <c r="EU3" s="71"/>
@@ -4040,28 +4050,29 @@
       <c r="FO3" s="71"/>
       <c r="FP3" s="71"/>
       <c r="FQ3" s="71"/>
-      <c r="FR3" s="72"/>
+      <c r="FR3" s="71"/>
       <c r="FS3" s="72"/>
-      <c r="FT3" s="71"/>
+      <c r="FT3" s="72"/>
       <c r="FU3" s="71"/>
       <c r="FV3" s="71"/>
-    </row>
-    <row r="4" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW3" s="71"/>
+    </row>
+    <row r="4" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
       <c r="D4" s="71"/>
       <c r="E4" s="71"/>
       <c r="F4" s="71"/>
       <c r="G4" s="71"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="73"/>
       <c r="J4" s="71"/>
       <c r="K4" s="71"/>
       <c r="L4" s="71"/>
       <c r="M4" s="71"/>
       <c r="N4" s="71"/>
-      <c r="O4" s="74"/>
-      <c r="P4" s="71"/>
+      <c r="O4" s="71"/>
+      <c r="P4" s="74"/>
       <c r="Q4" s="71"/>
       <c r="R4" s="71"/>
       <c r="S4" s="71"/>
@@ -4084,8 +4095,8 @@
       <c r="AJ4" s="71"/>
       <c r="AK4" s="71"/>
       <c r="AL4" s="71"/>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="71"/>
+      <c r="AM4" s="71"/>
+      <c r="AN4" s="74"/>
       <c r="AO4" s="71"/>
       <c r="AP4" s="71"/>
       <c r="AQ4" s="71"/>
@@ -4098,8 +4109,8 @@
       <c r="AX4" s="71"/>
       <c r="AY4" s="71"/>
       <c r="AZ4" s="71"/>
-      <c r="BA4" s="74"/>
-      <c r="BB4" s="71"/>
+      <c r="BA4" s="71"/>
+      <c r="BB4" s="74"/>
       <c r="BC4" s="71"/>
       <c r="BD4" s="71"/>
       <c r="BE4" s="71"/>
@@ -4137,8 +4148,8 @@
       <c r="CK4" s="71"/>
       <c r="CL4" s="71"/>
       <c r="CM4" s="71"/>
-      <c r="CN4" s="74"/>
-      <c r="CO4" s="71"/>
+      <c r="CN4" s="71"/>
+      <c r="CO4" s="74"/>
       <c r="CP4" s="71"/>
       <c r="CQ4" s="71"/>
       <c r="CR4" s="71"/>
@@ -4190,11 +4201,11 @@
       <c r="EL4" s="71"/>
       <c r="EM4" s="71"/>
       <c r="EN4" s="71"/>
-      <c r="EO4" s="74"/>
-      <c r="EP4" s="71"/>
+      <c r="EO4" s="71"/>
+      <c r="EP4" s="74"/>
       <c r="EQ4" s="71"/>
-      <c r="ER4" s="75"/>
-      <c r="ES4" s="71"/>
+      <c r="ER4" s="71"/>
+      <c r="ES4" s="75"/>
       <c r="ET4" s="71"/>
       <c r="EU4" s="71"/>
       <c r="EV4" s="71"/>
@@ -4224,23 +4235,32 @@
       <c r="FT4" s="71"/>
       <c r="FU4" s="71"/>
       <c r="FV4" s="71"/>
-    </row>
-    <row r="5" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW4" s="71"/>
+    </row>
+    <row r="5" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B5" s="71"/>
       <c r="C5" s="71"/>
       <c r="D5" s="71"/>
       <c r="E5" s="71"/>
       <c r="F5" s="71"/>
       <c r="G5" s="71"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
-      <c r="M5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="73"/>
+      <c r="J5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="K5" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="M5" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N5" s="71"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="71"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="74"/>
       <c r="Q5" s="71"/>
       <c r="R5" s="71"/>
       <c r="S5" s="71"/>
@@ -4263,8 +4283,8 @@
       <c r="AJ5" s="71"/>
       <c r="AK5" s="71"/>
       <c r="AL5" s="71"/>
-      <c r="AM5" s="74"/>
-      <c r="AN5" s="71"/>
+      <c r="AM5" s="71"/>
+      <c r="AN5" s="74"/>
       <c r="AO5" s="71"/>
       <c r="AP5" s="71"/>
       <c r="AQ5" s="71"/>
@@ -4277,8 +4297,8 @@
       <c r="AX5" s="71"/>
       <c r="AY5" s="71"/>
       <c r="AZ5" s="71"/>
-      <c r="BA5" s="74"/>
-      <c r="BB5" s="71"/>
+      <c r="BA5" s="71"/>
+      <c r="BB5" s="74"/>
       <c r="BC5" s="71"/>
       <c r="BD5" s="71"/>
       <c r="BE5" s="71"/>
@@ -4316,8 +4336,8 @@
       <c r="CK5" s="71"/>
       <c r="CL5" s="71"/>
       <c r="CM5" s="71"/>
-      <c r="CN5" s="74"/>
-      <c r="CO5" s="71"/>
+      <c r="CN5" s="71"/>
+      <c r="CO5" s="74"/>
       <c r="CP5" s="71"/>
       <c r="CQ5" s="71"/>
       <c r="CR5" s="71"/>
@@ -4369,11 +4389,11 @@
       <c r="EL5" s="71"/>
       <c r="EM5" s="71"/>
       <c r="EN5" s="71"/>
-      <c r="EO5" s="74"/>
-      <c r="EP5" s="71"/>
+      <c r="EO5" s="71"/>
+      <c r="EP5" s="74"/>
       <c r="EQ5" s="71"/>
-      <c r="ER5" s="75"/>
-      <c r="ES5" s="71"/>
+      <c r="ER5" s="71"/>
+      <c r="ES5" s="75"/>
       <c r="ET5" s="71"/>
       <c r="EU5" s="71"/>
       <c r="EV5" s="71"/>
@@ -4403,23 +4423,32 @@
       <c r="FT5" s="71"/>
       <c r="FU5" s="71"/>
       <c r="FV5" s="71"/>
-    </row>
-    <row r="6" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW5" s="71"/>
+    </row>
+    <row r="6" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B6" s="71"/>
       <c r="C6" s="71"/>
       <c r="D6" s="71"/>
       <c r="E6" s="71"/>
       <c r="F6" s="71"/>
       <c r="G6" s="71"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="K6" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="M6" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N6" s="71"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="71"/>
+      <c r="O6" s="71"/>
+      <c r="P6" s="74"/>
       <c r="Q6" s="71"/>
       <c r="R6" s="71"/>
       <c r="S6" s="71"/>
@@ -4442,8 +4471,8 @@
       <c r="AJ6" s="71"/>
       <c r="AK6" s="71"/>
       <c r="AL6" s="71"/>
-      <c r="AM6" s="74"/>
-      <c r="AN6" s="71"/>
+      <c r="AM6" s="71"/>
+      <c r="AN6" s="74"/>
       <c r="AO6" s="71"/>
       <c r="AP6" s="71"/>
       <c r="AQ6" s="71"/>
@@ -4456,8 +4485,8 @@
       <c r="AX6" s="71"/>
       <c r="AY6" s="71"/>
       <c r="AZ6" s="71"/>
-      <c r="BA6" s="74"/>
-      <c r="BB6" s="71"/>
+      <c r="BA6" s="71"/>
+      <c r="BB6" s="74"/>
       <c r="BC6" s="71"/>
       <c r="BD6" s="71"/>
       <c r="BE6" s="71"/>
@@ -4495,8 +4524,8 @@
       <c r="CK6" s="71"/>
       <c r="CL6" s="71"/>
       <c r="CM6" s="71"/>
-      <c r="CN6" s="74"/>
-      <c r="CO6" s="71"/>
+      <c r="CN6" s="71"/>
+      <c r="CO6" s="74"/>
       <c r="CP6" s="71"/>
       <c r="CQ6" s="71"/>
       <c r="CR6" s="71"/>
@@ -4548,11 +4577,11 @@
       <c r="EL6" s="71"/>
       <c r="EM6" s="71"/>
       <c r="EN6" s="71"/>
-      <c r="EO6" s="74"/>
-      <c r="EP6" s="71"/>
+      <c r="EO6" s="71"/>
+      <c r="EP6" s="74"/>
       <c r="EQ6" s="71"/>
-      <c r="ER6" s="75"/>
-      <c r="ES6" s="71"/>
+      <c r="ER6" s="71"/>
+      <c r="ES6" s="75"/>
       <c r="ET6" s="71"/>
       <c r="EU6" s="71"/>
       <c r="EV6" s="71"/>
@@ -4582,23 +4611,32 @@
       <c r="FT6" s="71"/>
       <c r="FU6" s="71"/>
       <c r="FV6" s="71"/>
-    </row>
-    <row r="7" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW6" s="71"/>
+    </row>
+    <row r="7" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B7" s="71"/>
       <c r="C7" s="71"/>
       <c r="D7" s="71"/>
       <c r="E7" s="71"/>
       <c r="F7" s="71"/>
       <c r="G7" s="71"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="K7" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="M7" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N7" s="71"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="74"/>
       <c r="Q7" s="71"/>
       <c r="R7" s="71"/>
       <c r="S7" s="71"/>
@@ -4621,8 +4659,8 @@
       <c r="AJ7" s="71"/>
       <c r="AK7" s="71"/>
       <c r="AL7" s="71"/>
-      <c r="AM7" s="74"/>
-      <c r="AN7" s="71"/>
+      <c r="AM7" s="71"/>
+      <c r="AN7" s="74"/>
       <c r="AO7" s="71"/>
       <c r="AP7" s="71"/>
       <c r="AQ7" s="71"/>
@@ -4635,8 +4673,8 @@
       <c r="AX7" s="71"/>
       <c r="AY7" s="71"/>
       <c r="AZ7" s="71"/>
-      <c r="BA7" s="74"/>
-      <c r="BB7" s="71"/>
+      <c r="BA7" s="71"/>
+      <c r="BB7" s="74"/>
       <c r="BC7" s="71"/>
       <c r="BD7" s="71"/>
       <c r="BE7" s="71"/>
@@ -4674,8 +4712,8 @@
       <c r="CK7" s="71"/>
       <c r="CL7" s="71"/>
       <c r="CM7" s="71"/>
-      <c r="CN7" s="74"/>
-      <c r="CO7" s="71"/>
+      <c r="CN7" s="71"/>
+      <c r="CO7" s="74"/>
       <c r="CP7" s="71"/>
       <c r="CQ7" s="71"/>
       <c r="CR7" s="71"/>
@@ -4727,11 +4765,11 @@
       <c r="EL7" s="71"/>
       <c r="EM7" s="71"/>
       <c r="EN7" s="71"/>
-      <c r="EO7" s="74"/>
-      <c r="EP7" s="71"/>
+      <c r="EO7" s="71"/>
+      <c r="EP7" s="74"/>
       <c r="EQ7" s="71"/>
-      <c r="ER7" s="75"/>
-      <c r="ES7" s="71"/>
+      <c r="ER7" s="71"/>
+      <c r="ES7" s="75"/>
       <c r="ET7" s="71"/>
       <c r="EU7" s="71"/>
       <c r="EV7" s="71"/>
@@ -4761,23 +4799,32 @@
       <c r="FT7" s="71"/>
       <c r="FU7" s="71"/>
       <c r="FV7" s="71"/>
-    </row>
-    <row r="8" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW7" s="71"/>
+    </row>
+    <row r="8" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B8" s="71"/>
       <c r="C8" s="71"/>
       <c r="D8" s="71"/>
       <c r="E8" s="71"/>
       <c r="F8" s="71"/>
       <c r="G8" s="71"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K8" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M8" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N8" s="71"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="74"/>
       <c r="Q8" s="71"/>
       <c r="R8" s="71"/>
       <c r="S8" s="71"/>
@@ -4800,8 +4847,8 @@
       <c r="AJ8" s="71"/>
       <c r="AK8" s="71"/>
       <c r="AL8" s="71"/>
-      <c r="AM8" s="74"/>
-      <c r="AN8" s="71"/>
+      <c r="AM8" s="71"/>
+      <c r="AN8" s="74"/>
       <c r="AO8" s="71"/>
       <c r="AP8" s="71"/>
       <c r="AQ8" s="71"/>
@@ -4814,8 +4861,8 @@
       <c r="AX8" s="71"/>
       <c r="AY8" s="71"/>
       <c r="AZ8" s="71"/>
-      <c r="BA8" s="74"/>
-      <c r="BB8" s="71"/>
+      <c r="BA8" s="71"/>
+      <c r="BB8" s="74"/>
       <c r="BC8" s="71"/>
       <c r="BD8" s="71"/>
       <c r="BE8" s="71"/>
@@ -4853,8 +4900,8 @@
       <c r="CK8" s="71"/>
       <c r="CL8" s="71"/>
       <c r="CM8" s="71"/>
-      <c r="CN8" s="74"/>
-      <c r="CO8" s="71"/>
+      <c r="CN8" s="71"/>
+      <c r="CO8" s="74"/>
       <c r="CP8" s="71"/>
       <c r="CQ8" s="71"/>
       <c r="CR8" s="71"/>
@@ -4906,11 +4953,11 @@
       <c r="EL8" s="71"/>
       <c r="EM8" s="71"/>
       <c r="EN8" s="71"/>
-      <c r="EO8" s="74"/>
-      <c r="EP8" s="71"/>
+      <c r="EO8" s="71"/>
+      <c r="EP8" s="74"/>
       <c r="EQ8" s="71"/>
-      <c r="ER8" s="75"/>
-      <c r="ES8" s="71"/>
+      <c r="ER8" s="71"/>
+      <c r="ES8" s="75"/>
       <c r="ET8" s="71"/>
       <c r="EU8" s="71"/>
       <c r="EV8" s="71"/>
@@ -4940,23 +4987,32 @@
       <c r="FT8" s="71"/>
       <c r="FU8" s="71"/>
       <c r="FV8" s="71"/>
-    </row>
-    <row r="9" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW8" s="71"/>
+    </row>
+    <row r="9" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B9" s="71"/>
       <c r="C9" s="71"/>
       <c r="D9" s="71"/>
       <c r="E9" s="71"/>
       <c r="F9" s="71"/>
       <c r="G9" s="71"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
-      <c r="L9" s="71"/>
-      <c r="M9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="K9" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="M9" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N9" s="71"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="71"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="74"/>
       <c r="Q9" s="71"/>
       <c r="R9" s="71"/>
       <c r="S9" s="71"/>
@@ -4979,8 +5035,8 @@
       <c r="AJ9" s="71"/>
       <c r="AK9" s="71"/>
       <c r="AL9" s="71"/>
-      <c r="AM9" s="74"/>
-      <c r="AN9" s="71"/>
+      <c r="AM9" s="71"/>
+      <c r="AN9" s="74"/>
       <c r="AO9" s="71"/>
       <c r="AP9" s="71"/>
       <c r="AQ9" s="71"/>
@@ -4993,8 +5049,8 @@
       <c r="AX9" s="71"/>
       <c r="AY9" s="71"/>
       <c r="AZ9" s="71"/>
-      <c r="BA9" s="74"/>
-      <c r="BB9" s="71"/>
+      <c r="BA9" s="71"/>
+      <c r="BB9" s="74"/>
       <c r="BC9" s="71"/>
       <c r="BD9" s="71"/>
       <c r="BE9" s="71"/>
@@ -5032,8 +5088,8 @@
       <c r="CK9" s="71"/>
       <c r="CL9" s="71"/>
       <c r="CM9" s="71"/>
-      <c r="CN9" s="74"/>
-      <c r="CO9" s="71"/>
+      <c r="CN9" s="71"/>
+      <c r="CO9" s="74"/>
       <c r="CP9" s="71"/>
       <c r="CQ9" s="71"/>
       <c r="CR9" s="71"/>
@@ -5085,11 +5141,11 @@
       <c r="EL9" s="71"/>
       <c r="EM9" s="71"/>
       <c r="EN9" s="71"/>
-      <c r="EO9" s="74"/>
-      <c r="EP9" s="71"/>
+      <c r="EO9" s="71"/>
+      <c r="EP9" s="74"/>
       <c r="EQ9" s="71"/>
-      <c r="ER9" s="75"/>
-      <c r="ES9" s="71"/>
+      <c r="ER9" s="71"/>
+      <c r="ES9" s="75"/>
       <c r="ET9" s="71"/>
       <c r="EU9" s="71"/>
       <c r="EV9" s="71"/>
@@ -5119,23 +5175,32 @@
       <c r="FT9" s="71"/>
       <c r="FU9" s="71"/>
       <c r="FV9" s="71"/>
-    </row>
-    <row r="10" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW9" s="71"/>
+    </row>
+    <row r="10" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B10" s="71"/>
       <c r="C10" s="71"/>
       <c r="D10" s="71"/>
       <c r="E10" s="71"/>
       <c r="F10" s="71"/>
       <c r="G10" s="71"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="73"/>
+      <c r="J10" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="K10" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="M10" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N10" s="71"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="71"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="74"/>
       <c r="Q10" s="71"/>
       <c r="R10" s="71"/>
       <c r="S10" s="71"/>
@@ -5158,8 +5223,8 @@
       <c r="AJ10" s="71"/>
       <c r="AK10" s="71"/>
       <c r="AL10" s="71"/>
-      <c r="AM10" s="74"/>
-      <c r="AN10" s="71"/>
+      <c r="AM10" s="71"/>
+      <c r="AN10" s="74"/>
       <c r="AO10" s="71"/>
       <c r="AP10" s="71"/>
       <c r="AQ10" s="71"/>
@@ -5172,8 +5237,8 @@
       <c r="AX10" s="71"/>
       <c r="AY10" s="71"/>
       <c r="AZ10" s="71"/>
-      <c r="BA10" s="74"/>
-      <c r="BB10" s="71"/>
+      <c r="BA10" s="71"/>
+      <c r="BB10" s="74"/>
       <c r="BC10" s="71"/>
       <c r="BD10" s="71"/>
       <c r="BE10" s="71"/>
@@ -5211,8 +5276,8 @@
       <c r="CK10" s="71"/>
       <c r="CL10" s="71"/>
       <c r="CM10" s="71"/>
-      <c r="CN10" s="74"/>
-      <c r="CO10" s="71"/>
+      <c r="CN10" s="71"/>
+      <c r="CO10" s="74"/>
       <c r="CP10" s="71"/>
       <c r="CQ10" s="71"/>
       <c r="CR10" s="71"/>
@@ -5264,11 +5329,11 @@
       <c r="EL10" s="71"/>
       <c r="EM10" s="71"/>
       <c r="EN10" s="71"/>
-      <c r="EO10" s="74"/>
-      <c r="EP10" s="71"/>
+      <c r="EO10" s="71"/>
+      <c r="EP10" s="74"/>
       <c r="EQ10" s="71"/>
-      <c r="ER10" s="75"/>
-      <c r="ES10" s="71"/>
+      <c r="ER10" s="71"/>
+      <c r="ES10" s="75"/>
       <c r="ET10" s="71"/>
       <c r="EU10" s="71"/>
       <c r="EV10" s="71"/>
@@ -5298,23 +5363,32 @@
       <c r="FT10" s="71"/>
       <c r="FU10" s="71"/>
       <c r="FV10" s="71"/>
-    </row>
-    <row r="11" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW10" s="71"/>
+    </row>
+    <row r="11" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B11" s="71"/>
       <c r="C11" s="71"/>
       <c r="D11" s="71"/>
       <c r="E11" s="71"/>
       <c r="F11" s="71"/>
       <c r="G11" s="71"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="K11" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="M11" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N11" s="71"/>
-      <c r="O11" s="74"/>
-      <c r="P11" s="71"/>
+      <c r="O11" s="71"/>
+      <c r="P11" s="74"/>
       <c r="Q11" s="71"/>
       <c r="R11" s="71"/>
       <c r="S11" s="71"/>
@@ -5337,8 +5411,8 @@
       <c r="AJ11" s="71"/>
       <c r="AK11" s="71"/>
       <c r="AL11" s="71"/>
-      <c r="AM11" s="74"/>
-      <c r="AN11" s="71"/>
+      <c r="AM11" s="71"/>
+      <c r="AN11" s="74"/>
       <c r="AO11" s="71"/>
       <c r="AP11" s="71"/>
       <c r="AQ11" s="71"/>
@@ -5351,8 +5425,8 @@
       <c r="AX11" s="71"/>
       <c r="AY11" s="71"/>
       <c r="AZ11" s="71"/>
-      <c r="BA11" s="74"/>
-      <c r="BB11" s="71"/>
+      <c r="BA11" s="71"/>
+      <c r="BB11" s="74"/>
       <c r="BC11" s="71"/>
       <c r="BD11" s="71"/>
       <c r="BE11" s="71"/>
@@ -5390,8 +5464,8 @@
       <c r="CK11" s="71"/>
       <c r="CL11" s="71"/>
       <c r="CM11" s="71"/>
-      <c r="CN11" s="74"/>
-      <c r="CO11" s="71"/>
+      <c r="CN11" s="71"/>
+      <c r="CO11" s="74"/>
       <c r="CP11" s="71"/>
       <c r="CQ11" s="71"/>
       <c r="CR11" s="71"/>
@@ -5443,11 +5517,11 @@
       <c r="EL11" s="71"/>
       <c r="EM11" s="71"/>
       <c r="EN11" s="71"/>
-      <c r="EO11" s="74"/>
-      <c r="EP11" s="71"/>
+      <c r="EO11" s="71"/>
+      <c r="EP11" s="74"/>
       <c r="EQ11" s="71"/>
-      <c r="ER11" s="75"/>
-      <c r="ES11" s="71"/>
+      <c r="ER11" s="71"/>
+      <c r="ES11" s="75"/>
       <c r="ET11" s="71"/>
       <c r="EU11" s="71"/>
       <c r="EV11" s="71"/>
@@ -5477,23 +5551,32 @@
       <c r="FT11" s="71"/>
       <c r="FU11" s="71"/>
       <c r="FV11" s="71"/>
-    </row>
-    <row r="12" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW11" s="71"/>
+    </row>
+    <row r="12" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B12" s="71"/>
       <c r="C12" s="71"/>
       <c r="D12" s="71"/>
       <c r="E12" s="71"/>
       <c r="F12" s="71"/>
       <c r="G12" s="71"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="K12" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="M12" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N12" s="71"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="74"/>
       <c r="Q12" s="71"/>
       <c r="R12" s="71"/>
       <c r="S12" s="71"/>
@@ -5516,8 +5599,8 @@
       <c r="AJ12" s="71"/>
       <c r="AK12" s="71"/>
       <c r="AL12" s="71"/>
-      <c r="AM12" s="74"/>
-      <c r="AN12" s="71"/>
+      <c r="AM12" s="71"/>
+      <c r="AN12" s="74"/>
       <c r="AO12" s="71"/>
       <c r="AP12" s="71"/>
       <c r="AQ12" s="71"/>
@@ -5530,8 +5613,8 @@
       <c r="AX12" s="71"/>
       <c r="AY12" s="71"/>
       <c r="AZ12" s="71"/>
-      <c r="BA12" s="74"/>
-      <c r="BB12" s="71"/>
+      <c r="BA12" s="71"/>
+      <c r="BB12" s="74"/>
       <c r="BC12" s="71"/>
       <c r="BD12" s="71"/>
       <c r="BE12" s="71"/>
@@ -5569,8 +5652,8 @@
       <c r="CK12" s="71"/>
       <c r="CL12" s="71"/>
       <c r="CM12" s="71"/>
-      <c r="CN12" s="74"/>
-      <c r="CO12" s="71"/>
+      <c r="CN12" s="71"/>
+      <c r="CO12" s="74"/>
       <c r="CP12" s="71"/>
       <c r="CQ12" s="71"/>
       <c r="CR12" s="71"/>
@@ -5622,11 +5705,11 @@
       <c r="EL12" s="71"/>
       <c r="EM12" s="71"/>
       <c r="EN12" s="71"/>
-      <c r="EO12" s="74"/>
-      <c r="EP12" s="71"/>
+      <c r="EO12" s="71"/>
+      <c r="EP12" s="74"/>
       <c r="EQ12" s="71"/>
-      <c r="ER12" s="75"/>
-      <c r="ES12" s="71"/>
+      <c r="ER12" s="71"/>
+      <c r="ES12" s="75"/>
       <c r="ET12" s="71"/>
       <c r="EU12" s="71"/>
       <c r="EV12" s="71"/>
@@ -5656,23 +5739,32 @@
       <c r="FT12" s="71"/>
       <c r="FU12" s="71"/>
       <c r="FV12" s="71"/>
-    </row>
-    <row r="13" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW12" s="71"/>
+    </row>
+    <row r="13" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B13" s="71"/>
       <c r="C13" s="71"/>
       <c r="D13" s="71"/>
       <c r="E13" s="71"/>
       <c r="F13" s="71"/>
       <c r="G13" s="71"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="K13" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="M13" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N13" s="71"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="71"/>
+      <c r="O13" s="71"/>
+      <c r="P13" s="74"/>
       <c r="Q13" s="71"/>
       <c r="R13" s="71"/>
       <c r="S13" s="71"/>
@@ -5695,8 +5787,8 @@
       <c r="AJ13" s="71"/>
       <c r="AK13" s="71"/>
       <c r="AL13" s="71"/>
-      <c r="AM13" s="74"/>
-      <c r="AN13" s="71"/>
+      <c r="AM13" s="71"/>
+      <c r="AN13" s="74"/>
       <c r="AO13" s="71"/>
       <c r="AP13" s="71"/>
       <c r="AQ13" s="71"/>
@@ -5709,8 +5801,8 @@
       <c r="AX13" s="71"/>
       <c r="AY13" s="71"/>
       <c r="AZ13" s="71"/>
-      <c r="BA13" s="74"/>
-      <c r="BB13" s="71"/>
+      <c r="BA13" s="71"/>
+      <c r="BB13" s="74"/>
       <c r="BC13" s="71"/>
       <c r="BD13" s="71"/>
       <c r="BE13" s="71"/>
@@ -5748,8 +5840,8 @@
       <c r="CK13" s="71"/>
       <c r="CL13" s="71"/>
       <c r="CM13" s="71"/>
-      <c r="CN13" s="74"/>
-      <c r="CO13" s="71"/>
+      <c r="CN13" s="71"/>
+      <c r="CO13" s="74"/>
       <c r="CP13" s="71"/>
       <c r="CQ13" s="71"/>
       <c r="CR13" s="71"/>
@@ -5801,11 +5893,11 @@
       <c r="EL13" s="71"/>
       <c r="EM13" s="71"/>
       <c r="EN13" s="71"/>
-      <c r="EO13" s="74"/>
-      <c r="EP13" s="71"/>
+      <c r="EO13" s="71"/>
+      <c r="EP13" s="74"/>
       <c r="EQ13" s="71"/>
-      <c r="ER13" s="75"/>
-      <c r="ES13" s="71"/>
+      <c r="ER13" s="71"/>
+      <c r="ES13" s="75"/>
       <c r="ET13" s="71"/>
       <c r="EU13" s="71"/>
       <c r="EV13" s="71"/>
@@ -5835,23 +5927,32 @@
       <c r="FT13" s="71"/>
       <c r="FU13" s="71"/>
       <c r="FV13" s="71"/>
-    </row>
-    <row r="14" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW13" s="71"/>
+    </row>
+    <row r="14" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B14" s="71"/>
       <c r="C14" s="71"/>
       <c r="D14" s="71"/>
       <c r="E14" s="71"/>
       <c r="F14" s="71"/>
       <c r="G14" s="71"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="K14" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="M14" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N14" s="71"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="71"/>
+      <c r="O14" s="71"/>
+      <c r="P14" s="74"/>
       <c r="Q14" s="71"/>
       <c r="R14" s="71"/>
       <c r="S14" s="71"/>
@@ -5874,8 +5975,8 @@
       <c r="AJ14" s="71"/>
       <c r="AK14" s="71"/>
       <c r="AL14" s="71"/>
-      <c r="AM14" s="74"/>
-      <c r="AN14" s="71"/>
+      <c r="AM14" s="71"/>
+      <c r="AN14" s="74"/>
       <c r="AO14" s="71"/>
       <c r="AP14" s="71"/>
       <c r="AQ14" s="71"/>
@@ -5888,8 +5989,8 @@
       <c r="AX14" s="71"/>
       <c r="AY14" s="71"/>
       <c r="AZ14" s="71"/>
-      <c r="BA14" s="74"/>
-      <c r="BB14" s="71"/>
+      <c r="BA14" s="71"/>
+      <c r="BB14" s="74"/>
       <c r="BC14" s="71"/>
       <c r="BD14" s="71"/>
       <c r="BE14" s="71"/>
@@ -5927,8 +6028,8 @@
       <c r="CK14" s="71"/>
       <c r="CL14" s="71"/>
       <c r="CM14" s="71"/>
-      <c r="CN14" s="74"/>
-      <c r="CO14" s="71"/>
+      <c r="CN14" s="71"/>
+      <c r="CO14" s="74"/>
       <c r="CP14" s="71"/>
       <c r="CQ14" s="71"/>
       <c r="CR14" s="71"/>
@@ -5980,11 +6081,11 @@
       <c r="EL14" s="71"/>
       <c r="EM14" s="71"/>
       <c r="EN14" s="71"/>
-      <c r="EO14" s="74"/>
-      <c r="EP14" s="71"/>
+      <c r="EO14" s="71"/>
+      <c r="EP14" s="74"/>
       <c r="EQ14" s="71"/>
-      <c r="ER14" s="75"/>
-      <c r="ES14" s="71"/>
+      <c r="ER14" s="71"/>
+      <c r="ES14" s="75"/>
       <c r="ET14" s="71"/>
       <c r="EU14" s="71"/>
       <c r="EV14" s="71"/>
@@ -6014,23 +6115,32 @@
       <c r="FT14" s="71"/>
       <c r="FU14" s="71"/>
       <c r="FV14" s="71"/>
-    </row>
-    <row r="15" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW14" s="71"/>
+    </row>
+    <row r="15" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B15" s="71"/>
       <c r="C15" s="71"/>
       <c r="D15" s="71"/>
       <c r="E15" s="71"/>
       <c r="F15" s="71"/>
       <c r="G15" s="71"/>
-      <c r="H15" s="73"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="71"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="K15" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="M15" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N15" s="71"/>
-      <c r="O15" s="74"/>
-      <c r="P15" s="71"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="74"/>
       <c r="Q15" s="71"/>
       <c r="R15" s="71"/>
       <c r="S15" s="71"/>
@@ -6053,8 +6163,8 @@
       <c r="AJ15" s="71"/>
       <c r="AK15" s="71"/>
       <c r="AL15" s="71"/>
-      <c r="AM15" s="74"/>
-      <c r="AN15" s="71"/>
+      <c r="AM15" s="71"/>
+      <c r="AN15" s="74"/>
       <c r="AO15" s="71"/>
       <c r="AP15" s="71"/>
       <c r="AQ15" s="71"/>
@@ -6067,8 +6177,8 @@
       <c r="AX15" s="71"/>
       <c r="AY15" s="71"/>
       <c r="AZ15" s="71"/>
-      <c r="BA15" s="74"/>
-      <c r="BB15" s="71"/>
+      <c r="BA15" s="71"/>
+      <c r="BB15" s="74"/>
       <c r="BC15" s="71"/>
       <c r="BD15" s="71"/>
       <c r="BE15" s="71"/>
@@ -6106,8 +6216,8 @@
       <c r="CK15" s="71"/>
       <c r="CL15" s="71"/>
       <c r="CM15" s="71"/>
-      <c r="CN15" s="74"/>
-      <c r="CO15" s="71"/>
+      <c r="CN15" s="71"/>
+      <c r="CO15" s="74"/>
       <c r="CP15" s="71"/>
       <c r="CQ15" s="71"/>
       <c r="CR15" s="71"/>
@@ -6159,11 +6269,11 @@
       <c r="EL15" s="71"/>
       <c r="EM15" s="71"/>
       <c r="EN15" s="71"/>
-      <c r="EO15" s="74"/>
-      <c r="EP15" s="71"/>
+      <c r="EO15" s="71"/>
+      <c r="EP15" s="74"/>
       <c r="EQ15" s="71"/>
-      <c r="ER15" s="75"/>
-      <c r="ES15" s="71"/>
+      <c r="ER15" s="71"/>
+      <c r="ES15" s="75"/>
       <c r="ET15" s="71"/>
       <c r="EU15" s="71"/>
       <c r="EV15" s="71"/>
@@ -6193,23 +6303,32 @@
       <c r="FT15" s="71"/>
       <c r="FU15" s="71"/>
       <c r="FV15" s="71"/>
-    </row>
-    <row r="16" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW15" s="71"/>
+    </row>
+    <row r="16" spans="2:179" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="71"/>
       <c r="C16" s="71"/>
       <c r="D16" s="71"/>
       <c r="E16" s="71"/>
       <c r="F16" s="71"/>
       <c r="G16" s="71"/>
-      <c r="H16" s="73"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="K16" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L16" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="M16" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N16" s="71"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="71"/>
+      <c r="O16" s="71"/>
+      <c r="P16" s="74"/>
       <c r="Q16" s="71"/>
       <c r="R16" s="71"/>
       <c r="S16" s="71"/>
@@ -6232,8 +6351,8 @@
       <c r="AJ16" s="71"/>
       <c r="AK16" s="71"/>
       <c r="AL16" s="71"/>
-      <c r="AM16" s="74"/>
-      <c r="AN16" s="71"/>
+      <c r="AM16" s="71"/>
+      <c r="AN16" s="74"/>
       <c r="AO16" s="71"/>
       <c r="AP16" s="71"/>
       <c r="AQ16" s="71"/>
@@ -6246,8 +6365,8 @@
       <c r="AX16" s="71"/>
       <c r="AY16" s="71"/>
       <c r="AZ16" s="71"/>
-      <c r="BA16" s="74"/>
-      <c r="BB16" s="71"/>
+      <c r="BA16" s="71"/>
+      <c r="BB16" s="74"/>
       <c r="BC16" s="71"/>
       <c r="BD16" s="71"/>
       <c r="BE16" s="71"/>
@@ -6285,8 +6404,8 @@
       <c r="CK16" s="71"/>
       <c r="CL16" s="71"/>
       <c r="CM16" s="71"/>
-      <c r="CN16" s="74"/>
-      <c r="CO16" s="71"/>
+      <c r="CN16" s="71"/>
+      <c r="CO16" s="74"/>
       <c r="CP16" s="71"/>
       <c r="CQ16" s="71"/>
       <c r="CR16" s="71"/>
@@ -6338,11 +6457,11 @@
       <c r="EL16" s="71"/>
       <c r="EM16" s="71"/>
       <c r="EN16" s="71"/>
-      <c r="EO16" s="74"/>
-      <c r="EP16" s="71"/>
+      <c r="EO16" s="71"/>
+      <c r="EP16" s="74"/>
       <c r="EQ16" s="71"/>
-      <c r="ER16" s="75"/>
-      <c r="ES16" s="71"/>
+      <c r="ER16" s="71"/>
+      <c r="ES16" s="75"/>
       <c r="ET16" s="71"/>
       <c r="EU16" s="71"/>
       <c r="EV16" s="71"/>
@@ -6372,23 +6491,28 @@
       <c r="FT16" s="71"/>
       <c r="FU16" s="71"/>
       <c r="FV16" s="71"/>
-    </row>
-    <row r="17" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW16" s="71"/>
+    </row>
+    <row r="17" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B17" s="71"/>
       <c r="C17" s="71"/>
       <c r="D17" s="71"/>
       <c r="E17" s="71"/>
       <c r="F17" s="71"/>
       <c r="G17" s="71"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L17" s="31"/>
+      <c r="M17" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N17" s="71"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="74"/>
       <c r="Q17" s="71"/>
       <c r="R17" s="71"/>
       <c r="S17" s="71"/>
@@ -6411,8 +6535,8 @@
       <c r="AJ17" s="71"/>
       <c r="AK17" s="71"/>
       <c r="AL17" s="71"/>
-      <c r="AM17" s="74"/>
-      <c r="AN17" s="71"/>
+      <c r="AM17" s="71"/>
+      <c r="AN17" s="74"/>
       <c r="AO17" s="71"/>
       <c r="AP17" s="71"/>
       <c r="AQ17" s="71"/>
@@ -6425,8 +6549,8 @@
       <c r="AX17" s="71"/>
       <c r="AY17" s="71"/>
       <c r="AZ17" s="71"/>
-      <c r="BA17" s="74"/>
-      <c r="BB17" s="71"/>
+      <c r="BA17" s="71"/>
+      <c r="BB17" s="74"/>
       <c r="BC17" s="71"/>
       <c r="BD17" s="71"/>
       <c r="BE17" s="71"/>
@@ -6464,8 +6588,8 @@
       <c r="CK17" s="71"/>
       <c r="CL17" s="71"/>
       <c r="CM17" s="71"/>
-      <c r="CN17" s="74"/>
-      <c r="CO17" s="71"/>
+      <c r="CN17" s="71"/>
+      <c r="CO17" s="74"/>
       <c r="CP17" s="71"/>
       <c r="CQ17" s="71"/>
       <c r="CR17" s="71"/>
@@ -6517,11 +6641,11 @@
       <c r="EL17" s="71"/>
       <c r="EM17" s="71"/>
       <c r="EN17" s="71"/>
-      <c r="EO17" s="74"/>
-      <c r="EP17" s="71"/>
+      <c r="EO17" s="71"/>
+      <c r="EP17" s="74"/>
       <c r="EQ17" s="71"/>
-      <c r="ER17" s="75"/>
-      <c r="ES17" s="71"/>
+      <c r="ER17" s="71"/>
+      <c r="ES17" s="75"/>
       <c r="ET17" s="71"/>
       <c r="EU17" s="71"/>
       <c r="EV17" s="71"/>
@@ -6551,23 +6675,28 @@
       <c r="FT17" s="71"/>
       <c r="FU17" s="71"/>
       <c r="FV17" s="71"/>
-    </row>
-    <row r="18" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW17" s="71"/>
+    </row>
+    <row r="18" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B18" s="71"/>
       <c r="C18" s="71"/>
       <c r="D18" s="71"/>
       <c r="E18" s="71"/>
       <c r="F18" s="71"/>
       <c r="G18" s="71"/>
-      <c r="H18" s="73"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L18" s="68"/>
+      <c r="M18" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N18" s="71"/>
-      <c r="O18" s="74"/>
-      <c r="P18" s="71"/>
+      <c r="O18" s="71"/>
+      <c r="P18" s="74"/>
       <c r="Q18" s="71"/>
       <c r="R18" s="71"/>
       <c r="S18" s="71"/>
@@ -6590,8 +6719,8 @@
       <c r="AJ18" s="71"/>
       <c r="AK18" s="71"/>
       <c r="AL18" s="71"/>
-      <c r="AM18" s="74"/>
-      <c r="AN18" s="71"/>
+      <c r="AM18" s="71"/>
+      <c r="AN18" s="74"/>
       <c r="AO18" s="71"/>
       <c r="AP18" s="71"/>
       <c r="AQ18" s="71"/>
@@ -6604,8 +6733,8 @@
       <c r="AX18" s="71"/>
       <c r="AY18" s="71"/>
       <c r="AZ18" s="71"/>
-      <c r="BA18" s="74"/>
-      <c r="BB18" s="71"/>
+      <c r="BA18" s="71"/>
+      <c r="BB18" s="74"/>
       <c r="BC18" s="71"/>
       <c r="BD18" s="71"/>
       <c r="BE18" s="71"/>
@@ -6643,8 +6772,8 @@
       <c r="CK18" s="71"/>
       <c r="CL18" s="71"/>
       <c r="CM18" s="71"/>
-      <c r="CN18" s="74"/>
-      <c r="CO18" s="71"/>
+      <c r="CN18" s="71"/>
+      <c r="CO18" s="74"/>
       <c r="CP18" s="71"/>
       <c r="CQ18" s="71"/>
       <c r="CR18" s="71"/>
@@ -6696,11 +6825,11 @@
       <c r="EL18" s="71"/>
       <c r="EM18" s="71"/>
       <c r="EN18" s="71"/>
-      <c r="EO18" s="74"/>
-      <c r="EP18" s="71"/>
+      <c r="EO18" s="71"/>
+      <c r="EP18" s="74"/>
       <c r="EQ18" s="71"/>
-      <c r="ER18" s="75"/>
-      <c r="ES18" s="71"/>
+      <c r="ER18" s="71"/>
+      <c r="ES18" s="75"/>
       <c r="ET18" s="71"/>
       <c r="EU18" s="71"/>
       <c r="EV18" s="71"/>
@@ -6730,23 +6859,28 @@
       <c r="FT18" s="71"/>
       <c r="FU18" s="71"/>
       <c r="FV18" s="71"/>
-    </row>
-    <row r="19" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW18" s="71"/>
+    </row>
+    <row r="19" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B19" s="71"/>
       <c r="C19" s="71"/>
       <c r="D19" s="71"/>
       <c r="E19" s="71"/>
       <c r="F19" s="71"/>
       <c r="G19" s="71"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="71"/>
-      <c r="J19" s="71"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="71"/>
-      <c r="M19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L19" s="78"/>
+      <c r="M19" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N19" s="71"/>
-      <c r="O19" s="74"/>
-      <c r="P19" s="71"/>
+      <c r="O19" s="71"/>
+      <c r="P19" s="74"/>
       <c r="Q19" s="71"/>
       <c r="R19" s="71"/>
       <c r="S19" s="71"/>
@@ -6769,8 +6903,8 @@
       <c r="AJ19" s="71"/>
       <c r="AK19" s="71"/>
       <c r="AL19" s="71"/>
-      <c r="AM19" s="74"/>
-      <c r="AN19" s="71"/>
+      <c r="AM19" s="71"/>
+      <c r="AN19" s="74"/>
       <c r="AO19" s="71"/>
       <c r="AP19" s="71"/>
       <c r="AQ19" s="71"/>
@@ -6783,8 +6917,8 @@
       <c r="AX19" s="71"/>
       <c r="AY19" s="71"/>
       <c r="AZ19" s="71"/>
-      <c r="BA19" s="74"/>
-      <c r="BB19" s="71"/>
+      <c r="BA19" s="71"/>
+      <c r="BB19" s="74"/>
       <c r="BC19" s="71"/>
       <c r="BD19" s="71"/>
       <c r="BE19" s="71"/>
@@ -6822,8 +6956,8 @@
       <c r="CK19" s="71"/>
       <c r="CL19" s="71"/>
       <c r="CM19" s="71"/>
-      <c r="CN19" s="74"/>
-      <c r="CO19" s="71"/>
+      <c r="CN19" s="71"/>
+      <c r="CO19" s="74"/>
       <c r="CP19" s="71"/>
       <c r="CQ19" s="71"/>
       <c r="CR19" s="71"/>
@@ -6875,11 +7009,11 @@
       <c r="EL19" s="71"/>
       <c r="EM19" s="71"/>
       <c r="EN19" s="71"/>
-      <c r="EO19" s="74"/>
-      <c r="EP19" s="71"/>
+      <c r="EO19" s="71"/>
+      <c r="EP19" s="74"/>
       <c r="EQ19" s="71"/>
-      <c r="ER19" s="75"/>
-      <c r="ES19" s="71"/>
+      <c r="ER19" s="71"/>
+      <c r="ES19" s="75"/>
       <c r="ET19" s="71"/>
       <c r="EU19" s="71"/>
       <c r="EV19" s="71"/>
@@ -6909,23 +7043,28 @@
       <c r="FT19" s="71"/>
       <c r="FU19" s="71"/>
       <c r="FV19" s="71"/>
-    </row>
-    <row r="20" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW19" s="71"/>
+    </row>
+    <row r="20" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B20" s="71"/>
       <c r="C20" s="71"/>
       <c r="D20" s="71"/>
       <c r="E20" s="71"/>
       <c r="F20" s="71"/>
       <c r="G20" s="71"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="71"/>
-      <c r="M20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L20" s="78"/>
+      <c r="M20" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N20" s="71"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="71"/>
+      <c r="O20" s="71"/>
+      <c r="P20" s="74"/>
       <c r="Q20" s="71"/>
       <c r="R20" s="71"/>
       <c r="S20" s="71"/>
@@ -6948,8 +7087,8 @@
       <c r="AJ20" s="71"/>
       <c r="AK20" s="71"/>
       <c r="AL20" s="71"/>
-      <c r="AM20" s="74"/>
-      <c r="AN20" s="71"/>
+      <c r="AM20" s="71"/>
+      <c r="AN20" s="74"/>
       <c r="AO20" s="71"/>
       <c r="AP20" s="71"/>
       <c r="AQ20" s="71"/>
@@ -6962,8 +7101,8 @@
       <c r="AX20" s="71"/>
       <c r="AY20" s="71"/>
       <c r="AZ20" s="71"/>
-      <c r="BA20" s="74"/>
-      <c r="BB20" s="71"/>
+      <c r="BA20" s="71"/>
+      <c r="BB20" s="74"/>
       <c r="BC20" s="71"/>
       <c r="BD20" s="71"/>
       <c r="BE20" s="71"/>
@@ -7001,8 +7140,8 @@
       <c r="CK20" s="71"/>
       <c r="CL20" s="71"/>
       <c r="CM20" s="71"/>
-      <c r="CN20" s="74"/>
-      <c r="CO20" s="71"/>
+      <c r="CN20" s="71"/>
+      <c r="CO20" s="74"/>
       <c r="CP20" s="71"/>
       <c r="CQ20" s="71"/>
       <c r="CR20" s="71"/>
@@ -7054,11 +7193,11 @@
       <c r="EL20" s="71"/>
       <c r="EM20" s="71"/>
       <c r="EN20" s="71"/>
-      <c r="EO20" s="74"/>
-      <c r="EP20" s="71"/>
+      <c r="EO20" s="71"/>
+      <c r="EP20" s="74"/>
       <c r="EQ20" s="71"/>
-      <c r="ER20" s="75"/>
-      <c r="ES20" s="71"/>
+      <c r="ER20" s="71"/>
+      <c r="ES20" s="75"/>
       <c r="ET20" s="71"/>
       <c r="EU20" s="71"/>
       <c r="EV20" s="71"/>
@@ -7088,23 +7227,28 @@
       <c r="FT20" s="71"/>
       <c r="FU20" s="71"/>
       <c r="FV20" s="71"/>
-    </row>
-    <row r="21" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW20" s="71"/>
+    </row>
+    <row r="21" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B21" s="71"/>
       <c r="C21" s="71"/>
       <c r="D21" s="71"/>
       <c r="E21" s="71"/>
       <c r="F21" s="71"/>
       <c r="G21" s="71"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="71"/>
-      <c r="M21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="73"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L21" s="78"/>
+      <c r="M21" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N21" s="71"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="71"/>
+      <c r="O21" s="71"/>
+      <c r="P21" s="74"/>
       <c r="Q21" s="71"/>
       <c r="R21" s="71"/>
       <c r="S21" s="71"/>
@@ -7127,8 +7271,8 @@
       <c r="AJ21" s="71"/>
       <c r="AK21" s="71"/>
       <c r="AL21" s="71"/>
-      <c r="AM21" s="74"/>
-      <c r="AN21" s="71"/>
+      <c r="AM21" s="71"/>
+      <c r="AN21" s="74"/>
       <c r="AO21" s="71"/>
       <c r="AP21" s="71"/>
       <c r="AQ21" s="71"/>
@@ -7141,8 +7285,8 @@
       <c r="AX21" s="71"/>
       <c r="AY21" s="71"/>
       <c r="AZ21" s="71"/>
-      <c r="BA21" s="74"/>
-      <c r="BB21" s="71"/>
+      <c r="BA21" s="71"/>
+      <c r="BB21" s="74"/>
       <c r="BC21" s="71"/>
       <c r="BD21" s="71"/>
       <c r="BE21" s="71"/>
@@ -7180,8 +7324,8 @@
       <c r="CK21" s="71"/>
       <c r="CL21" s="71"/>
       <c r="CM21" s="71"/>
-      <c r="CN21" s="74"/>
-      <c r="CO21" s="71"/>
+      <c r="CN21" s="71"/>
+      <c r="CO21" s="74"/>
       <c r="CP21" s="71"/>
       <c r="CQ21" s="71"/>
       <c r="CR21" s="71"/>
@@ -7233,11 +7377,11 @@
       <c r="EL21" s="71"/>
       <c r="EM21" s="71"/>
       <c r="EN21" s="71"/>
-      <c r="EO21" s="74"/>
-      <c r="EP21" s="71"/>
+      <c r="EO21" s="71"/>
+      <c r="EP21" s="74"/>
       <c r="EQ21" s="71"/>
-      <c r="ER21" s="75"/>
-      <c r="ES21" s="71"/>
+      <c r="ER21" s="71"/>
+      <c r="ES21" s="75"/>
       <c r="ET21" s="71"/>
       <c r="EU21" s="71"/>
       <c r="EV21" s="71"/>
@@ -7267,23 +7411,28 @@
       <c r="FT21" s="71"/>
       <c r="FU21" s="71"/>
       <c r="FV21" s="71"/>
-    </row>
-    <row r="22" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW21" s="71"/>
+    </row>
+    <row r="22" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B22" s="71"/>
       <c r="C22" s="71"/>
       <c r="D22" s="71"/>
       <c r="E22" s="71"/>
       <c r="F22" s="71"/>
       <c r="G22" s="71"/>
-      <c r="H22" s="73"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L22" s="78"/>
+      <c r="M22" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N22" s="71"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="71"/>
+      <c r="O22" s="71"/>
+      <c r="P22" s="74"/>
       <c r="Q22" s="71"/>
       <c r="R22" s="71"/>
       <c r="S22" s="71"/>
@@ -7306,8 +7455,8 @@
       <c r="AJ22" s="71"/>
       <c r="AK22" s="71"/>
       <c r="AL22" s="71"/>
-      <c r="AM22" s="74"/>
-      <c r="AN22" s="71"/>
+      <c r="AM22" s="71"/>
+      <c r="AN22" s="74"/>
       <c r="AO22" s="71"/>
       <c r="AP22" s="71"/>
       <c r="AQ22" s="71"/>
@@ -7320,8 +7469,8 @@
       <c r="AX22" s="71"/>
       <c r="AY22" s="71"/>
       <c r="AZ22" s="71"/>
-      <c r="BA22" s="74"/>
-      <c r="BB22" s="71"/>
+      <c r="BA22" s="71"/>
+      <c r="BB22" s="74"/>
       <c r="BC22" s="71"/>
       <c r="BD22" s="71"/>
       <c r="BE22" s="71"/>
@@ -7359,8 +7508,8 @@
       <c r="CK22" s="71"/>
       <c r="CL22" s="71"/>
       <c r="CM22" s="71"/>
-      <c r="CN22" s="74"/>
-      <c r="CO22" s="71"/>
+      <c r="CN22" s="71"/>
+      <c r="CO22" s="74"/>
       <c r="CP22" s="71"/>
       <c r="CQ22" s="71"/>
       <c r="CR22" s="71"/>
@@ -7412,11 +7561,11 @@
       <c r="EL22" s="71"/>
       <c r="EM22" s="71"/>
       <c r="EN22" s="71"/>
-      <c r="EO22" s="74"/>
-      <c r="EP22" s="71"/>
+      <c r="EO22" s="71"/>
+      <c r="EP22" s="74"/>
       <c r="EQ22" s="71"/>
-      <c r="ER22" s="75"/>
-      <c r="ES22" s="71"/>
+      <c r="ER22" s="71"/>
+      <c r="ES22" s="75"/>
       <c r="ET22" s="71"/>
       <c r="EU22" s="71"/>
       <c r="EV22" s="71"/>
@@ -7446,23 +7595,28 @@
       <c r="FT22" s="71"/>
       <c r="FU22" s="71"/>
       <c r="FV22" s="71"/>
-    </row>
-    <row r="23" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW22" s="71"/>
+    </row>
+    <row r="23" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B23" s="71"/>
       <c r="C23" s="71"/>
       <c r="D23" s="71"/>
       <c r="E23" s="71"/>
       <c r="F23" s="71"/>
       <c r="G23" s="71"/>
-      <c r="H23" s="73"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="73"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L23" s="78"/>
+      <c r="M23" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N23" s="71"/>
-      <c r="O23" s="74"/>
-      <c r="P23" s="71"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="74"/>
       <c r="Q23" s="71"/>
       <c r="R23" s="71"/>
       <c r="S23" s="71"/>
@@ -7485,8 +7639,8 @@
       <c r="AJ23" s="71"/>
       <c r="AK23" s="71"/>
       <c r="AL23" s="71"/>
-      <c r="AM23" s="74"/>
-      <c r="AN23" s="71"/>
+      <c r="AM23" s="71"/>
+      <c r="AN23" s="74"/>
       <c r="AO23" s="71"/>
       <c r="AP23" s="71"/>
       <c r="AQ23" s="71"/>
@@ -7499,8 +7653,8 @@
       <c r="AX23" s="71"/>
       <c r="AY23" s="71"/>
       <c r="AZ23" s="71"/>
-      <c r="BA23" s="74"/>
-      <c r="BB23" s="71"/>
+      <c r="BA23" s="71"/>
+      <c r="BB23" s="74"/>
       <c r="BC23" s="71"/>
       <c r="BD23" s="71"/>
       <c r="BE23" s="71"/>
@@ -7538,8 +7692,8 @@
       <c r="CK23" s="71"/>
       <c r="CL23" s="71"/>
       <c r="CM23" s="71"/>
-      <c r="CN23" s="74"/>
-      <c r="CO23" s="71"/>
+      <c r="CN23" s="71"/>
+      <c r="CO23" s="74"/>
       <c r="CP23" s="71"/>
       <c r="CQ23" s="71"/>
       <c r="CR23" s="71"/>
@@ -7591,11 +7745,11 @@
       <c r="EL23" s="71"/>
       <c r="EM23" s="71"/>
       <c r="EN23" s="71"/>
-      <c r="EO23" s="74"/>
-      <c r="EP23" s="71"/>
+      <c r="EO23" s="71"/>
+      <c r="EP23" s="74"/>
       <c r="EQ23" s="71"/>
-      <c r="ER23" s="75"/>
-      <c r="ES23" s="71"/>
+      <c r="ER23" s="71"/>
+      <c r="ES23" s="75"/>
       <c r="ET23" s="71"/>
       <c r="EU23" s="71"/>
       <c r="EV23" s="71"/>
@@ -7625,23 +7779,28 @@
       <c r="FT23" s="71"/>
       <c r="FU23" s="71"/>
       <c r="FV23" s="71"/>
-    </row>
-    <row r="24" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW23" s="71"/>
+    </row>
+    <row r="24" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B24" s="71"/>
       <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="78"/>
       <c r="G24" s="71"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="71"/>
-      <c r="K24" s="71"/>
-      <c r="L24" s="71"/>
-      <c r="M24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L24" s="78"/>
+      <c r="M24" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N24" s="71"/>
-      <c r="O24" s="74"/>
-      <c r="P24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="74"/>
       <c r="Q24" s="71"/>
       <c r="R24" s="71"/>
       <c r="S24" s="71"/>
@@ -7664,8 +7823,8 @@
       <c r="AJ24" s="71"/>
       <c r="AK24" s="71"/>
       <c r="AL24" s="71"/>
-      <c r="AM24" s="74"/>
-      <c r="AN24" s="71"/>
+      <c r="AM24" s="71"/>
+      <c r="AN24" s="74"/>
       <c r="AO24" s="71"/>
       <c r="AP24" s="71"/>
       <c r="AQ24" s="71"/>
@@ -7678,8 +7837,8 @@
       <c r="AX24" s="71"/>
       <c r="AY24" s="71"/>
       <c r="AZ24" s="71"/>
-      <c r="BA24" s="74"/>
-      <c r="BB24" s="71"/>
+      <c r="BA24" s="71"/>
+      <c r="BB24" s="74"/>
       <c r="BC24" s="71"/>
       <c r="BD24" s="71"/>
       <c r="BE24" s="71"/>
@@ -7717,8 +7876,8 @@
       <c r="CK24" s="71"/>
       <c r="CL24" s="71"/>
       <c r="CM24" s="71"/>
-      <c r="CN24" s="74"/>
-      <c r="CO24" s="71"/>
+      <c r="CN24" s="71"/>
+      <c r="CO24" s="74"/>
       <c r="CP24" s="71"/>
       <c r="CQ24" s="71"/>
       <c r="CR24" s="71"/>
@@ -7770,11 +7929,11 @@
       <c r="EL24" s="71"/>
       <c r="EM24" s="71"/>
       <c r="EN24" s="71"/>
-      <c r="EO24" s="74"/>
-      <c r="EP24" s="71"/>
+      <c r="EO24" s="71"/>
+      <c r="EP24" s="74"/>
       <c r="EQ24" s="71"/>
-      <c r="ER24" s="75"/>
-      <c r="ES24" s="71"/>
+      <c r="ER24" s="71"/>
+      <c r="ES24" s="75"/>
       <c r="ET24" s="71"/>
       <c r="EU24" s="71"/>
       <c r="EV24" s="71"/>
@@ -7804,23 +7963,28 @@
       <c r="FT24" s="71"/>
       <c r="FU24" s="71"/>
       <c r="FV24" s="71"/>
-    </row>
-    <row r="25" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW24" s="71"/>
+    </row>
+    <row r="25" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B25" s="71"/>
       <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
       <c r="G25" s="71"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="71"/>
-      <c r="J25" s="71"/>
-      <c r="K25" s="71"/>
-      <c r="L25" s="71"/>
-      <c r="M25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L25" s="78"/>
+      <c r="M25" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N25" s="71"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="74"/>
       <c r="Q25" s="71"/>
       <c r="R25" s="71"/>
       <c r="S25" s="71"/>
@@ -7843,8 +8007,8 @@
       <c r="AJ25" s="71"/>
       <c r="AK25" s="71"/>
       <c r="AL25" s="71"/>
-      <c r="AM25" s="74"/>
-      <c r="AN25" s="71"/>
+      <c r="AM25" s="71"/>
+      <c r="AN25" s="74"/>
       <c r="AO25" s="71"/>
       <c r="AP25" s="71"/>
       <c r="AQ25" s="71"/>
@@ -7857,8 +8021,8 @@
       <c r="AX25" s="71"/>
       <c r="AY25" s="71"/>
       <c r="AZ25" s="71"/>
-      <c r="BA25" s="74"/>
-      <c r="BB25" s="71"/>
+      <c r="BA25" s="71"/>
+      <c r="BB25" s="74"/>
       <c r="BC25" s="71"/>
       <c r="BD25" s="71"/>
       <c r="BE25" s="71"/>
@@ -7896,8 +8060,8 @@
       <c r="CK25" s="71"/>
       <c r="CL25" s="71"/>
       <c r="CM25" s="71"/>
-      <c r="CN25" s="74"/>
-      <c r="CO25" s="71"/>
+      <c r="CN25" s="71"/>
+      <c r="CO25" s="74"/>
       <c r="CP25" s="71"/>
       <c r="CQ25" s="71"/>
       <c r="CR25" s="71"/>
@@ -7949,11 +8113,11 @@
       <c r="EL25" s="71"/>
       <c r="EM25" s="71"/>
       <c r="EN25" s="71"/>
-      <c r="EO25" s="74"/>
-      <c r="EP25" s="71"/>
+      <c r="EO25" s="71"/>
+      <c r="EP25" s="74"/>
       <c r="EQ25" s="71"/>
-      <c r="ER25" s="75"/>
-      <c r="ES25" s="71"/>
+      <c r="ER25" s="71"/>
+      <c r="ES25" s="75"/>
       <c r="ET25" s="71"/>
       <c r="EU25" s="71"/>
       <c r="EV25" s="71"/>
@@ -7983,23 +8147,28 @@
       <c r="FT25" s="71"/>
       <c r="FU25" s="71"/>
       <c r="FV25" s="71"/>
-    </row>
-    <row r="26" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW25" s="71"/>
+    </row>
+    <row r="26" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B26" s="71"/>
       <c r="C26" s="71"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="71"/>
-      <c r="F26" s="71"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
       <c r="G26" s="71"/>
-      <c r="H26" s="73"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="71"/>
-      <c r="L26" s="71"/>
-      <c r="M26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L26" s="78"/>
+      <c r="M26" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N26" s="71"/>
-      <c r="O26" s="74"/>
-      <c r="P26" s="71"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="74"/>
       <c r="Q26" s="71"/>
       <c r="R26" s="71"/>
       <c r="S26" s="71"/>
@@ -8022,8 +8191,8 @@
       <c r="AJ26" s="71"/>
       <c r="AK26" s="71"/>
       <c r="AL26" s="71"/>
-      <c r="AM26" s="74"/>
-      <c r="AN26" s="71"/>
+      <c r="AM26" s="71"/>
+      <c r="AN26" s="74"/>
       <c r="AO26" s="71"/>
       <c r="AP26" s="71"/>
       <c r="AQ26" s="71"/>
@@ -8036,8 +8205,8 @@
       <c r="AX26" s="71"/>
       <c r="AY26" s="71"/>
       <c r="AZ26" s="71"/>
-      <c r="BA26" s="74"/>
-      <c r="BB26" s="71"/>
+      <c r="BA26" s="71"/>
+      <c r="BB26" s="74"/>
       <c r="BC26" s="71"/>
       <c r="BD26" s="71"/>
       <c r="BE26" s="71"/>
@@ -8075,8 +8244,8 @@
       <c r="CK26" s="71"/>
       <c r="CL26" s="71"/>
       <c r="CM26" s="71"/>
-      <c r="CN26" s="74"/>
-      <c r="CO26" s="71"/>
+      <c r="CN26" s="71"/>
+      <c r="CO26" s="74"/>
       <c r="CP26" s="71"/>
       <c r="CQ26" s="71"/>
       <c r="CR26" s="71"/>
@@ -8128,11 +8297,11 @@
       <c r="EL26" s="71"/>
       <c r="EM26" s="71"/>
       <c r="EN26" s="71"/>
-      <c r="EO26" s="74"/>
-      <c r="EP26" s="71"/>
+      <c r="EO26" s="71"/>
+      <c r="EP26" s="74"/>
       <c r="EQ26" s="71"/>
-      <c r="ER26" s="75"/>
-      <c r="ES26" s="71"/>
+      <c r="ER26" s="71"/>
+      <c r="ES26" s="75"/>
       <c r="ET26" s="71"/>
       <c r="EU26" s="71"/>
       <c r="EV26" s="71"/>
@@ -8162,23 +8331,28 @@
       <c r="FT26" s="71"/>
       <c r="FU26" s="71"/>
       <c r="FV26" s="71"/>
-    </row>
-    <row r="27" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW26" s="71"/>
+    </row>
+    <row r="27" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B27" s="71"/>
       <c r="C27" s="71"/>
-      <c r="D27" s="71"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="71"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
       <c r="G27" s="71"/>
-      <c r="H27" s="73"/>
-      <c r="I27" s="71"/>
-      <c r="J27" s="71"/>
-      <c r="K27" s="71"/>
-      <c r="L27" s="71"/>
-      <c r="M27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L27" s="78"/>
+      <c r="M27" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N27" s="71"/>
-      <c r="O27" s="74"/>
-      <c r="P27" s="71"/>
+      <c r="O27" s="71"/>
+      <c r="P27" s="74"/>
       <c r="Q27" s="71"/>
       <c r="R27" s="71"/>
       <c r="S27" s="71"/>
@@ -8201,8 +8375,8 @@
       <c r="AJ27" s="71"/>
       <c r="AK27" s="71"/>
       <c r="AL27" s="71"/>
-      <c r="AM27" s="74"/>
-      <c r="AN27" s="71"/>
+      <c r="AM27" s="71"/>
+      <c r="AN27" s="74"/>
       <c r="AO27" s="71"/>
       <c r="AP27" s="71"/>
       <c r="AQ27" s="71"/>
@@ -8215,8 +8389,8 @@
       <c r="AX27" s="71"/>
       <c r="AY27" s="71"/>
       <c r="AZ27" s="71"/>
-      <c r="BA27" s="74"/>
-      <c r="BB27" s="71"/>
+      <c r="BA27" s="71"/>
+      <c r="BB27" s="74"/>
       <c r="BC27" s="71"/>
       <c r="BD27" s="71"/>
       <c r="BE27" s="71"/>
@@ -8254,8 +8428,8 @@
       <c r="CK27" s="71"/>
       <c r="CL27" s="71"/>
       <c r="CM27" s="71"/>
-      <c r="CN27" s="74"/>
-      <c r="CO27" s="71"/>
+      <c r="CN27" s="71"/>
+      <c r="CO27" s="74"/>
       <c r="CP27" s="71"/>
       <c r="CQ27" s="71"/>
       <c r="CR27" s="71"/>
@@ -8307,11 +8481,11 @@
       <c r="EL27" s="71"/>
       <c r="EM27" s="71"/>
       <c r="EN27" s="71"/>
-      <c r="EO27" s="74"/>
-      <c r="EP27" s="71"/>
+      <c r="EO27" s="71"/>
+      <c r="EP27" s="74"/>
       <c r="EQ27" s="71"/>
-      <c r="ER27" s="75"/>
-      <c r="ES27" s="71"/>
+      <c r="ER27" s="71"/>
+      <c r="ES27" s="75"/>
       <c r="ET27" s="71"/>
       <c r="EU27" s="71"/>
       <c r="EV27" s="71"/>
@@ -8341,23 +8515,28 @@
       <c r="FT27" s="71"/>
       <c r="FU27" s="71"/>
       <c r="FV27" s="71"/>
-    </row>
-    <row r="28" spans="2:178" x14ac:dyDescent="0.25">
+      <c r="FW27" s="71"/>
+    </row>
+    <row r="28" spans="2:179" x14ac:dyDescent="0.25">
       <c r="B28" s="71"/>
       <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
       <c r="G28" s="71"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="71"/>
-      <c r="K28" s="71"/>
-      <c r="L28" s="71"/>
-      <c r="M28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L28" s="78"/>
+      <c r="M28" s="71" t="s">
+        <v>270</v>
+      </c>
       <c r="N28" s="71"/>
-      <c r="O28" s="74"/>
-      <c r="P28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="74"/>
       <c r="Q28" s="71"/>
       <c r="R28" s="71"/>
       <c r="S28" s="71"/>
@@ -8380,8 +8559,8 @@
       <c r="AJ28" s="71"/>
       <c r="AK28" s="71"/>
       <c r="AL28" s="71"/>
-      <c r="AM28" s="74"/>
-      <c r="AN28" s="71"/>
+      <c r="AM28" s="71"/>
+      <c r="AN28" s="74"/>
       <c r="AO28" s="71"/>
       <c r="AP28" s="71"/>
       <c r="AQ28" s="71"/>
@@ -8394,8 +8573,8 @@
       <c r="AX28" s="71"/>
       <c r="AY28" s="71"/>
       <c r="AZ28" s="71"/>
-      <c r="BA28" s="74"/>
-      <c r="BB28" s="71"/>
+      <c r="BA28" s="71"/>
+      <c r="BB28" s="74"/>
       <c r="BC28" s="71"/>
       <c r="BD28" s="71"/>
       <c r="BE28" s="71"/>
@@ -8433,8 +8612,8 @@
       <c r="CK28" s="71"/>
       <c r="CL28" s="71"/>
       <c r="CM28" s="71"/>
-      <c r="CN28" s="74"/>
-      <c r="CO28" s="71"/>
+      <c r="CN28" s="71"/>
+      <c r="CO28" s="74"/>
       <c r="CP28" s="71"/>
       <c r="CQ28" s="71"/>
       <c r="CR28" s="71"/>
@@ -8486,11 +8665,11 @@
       <c r="EL28" s="71"/>
       <c r="EM28" s="71"/>
       <c r="EN28" s="71"/>
-      <c r="EO28" s="74"/>
-      <c r="EP28" s="71"/>
+      <c r="EO28" s="71"/>
+      <c r="EP28" s="74"/>
       <c r="EQ28" s="71"/>
-      <c r="ER28" s="75"/>
-      <c r="ES28" s="71"/>
+      <c r="ER28" s="71"/>
+      <c r="ES28" s="75"/>
       <c r="ET28" s="71"/>
       <c r="EU28" s="71"/>
       <c r="EV28" s="71"/>
@@ -8520,6 +8699,49 @@
       <c r="FT28" s="71"/>
       <c r="FU28" s="71"/>
       <c r="FV28" s="71"/>
+      <c r="FW28" s="71"/>
+    </row>
+    <row r="29" spans="2:179" x14ac:dyDescent="0.25">
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="71"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L29" s="78"/>
+      <c r="M29" s="71" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="30" spans="2:179" x14ac:dyDescent="0.25">
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="71"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L30" s="78"/>
+      <c r="M30" s="71" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="31" spans="2:179" x14ac:dyDescent="0.25">
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="71"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="71" t="s">
+        <v>269</v>
+      </c>
+      <c r="L31" s="78"/>
+      <c r="M31" s="71" t="s">
+        <v>270</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>

</xml_diff>

<commit_message>
Drobne korekty w okolicach danych wariantowych
git-svn-id: https://localhost:8443/svn/bdr@1016 5173494c-6dae-45e1-bfb1-e08744c75a4d
</commit_message>
<xml_diff>
--- a/TPP/dokumenty/TPP_atrybuty1.xlsx
+++ b/TPP/dokumenty/TPP_atrybuty1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="314">
   <si>
     <t>Nazwa atrybutu</t>
   </si>
@@ -703,9 +703,6 @@
   </si>
   <si>
     <t>MotionAnalysis</t>
-  </si>
-  <si>
-    <t>DBSAktywna</t>
   </si>
   <si>
     <t>BadanieWechu</t>
@@ -850,6 +847,129 @@
   </si>
   <si>
     <t>0=brak okna; 1=brak hyperechogeniczności; 2=hyperechogeniczność</t>
+  </si>
+  <si>
+    <t>DBS</t>
+  </si>
+  <si>
+    <t>@DBS,</t>
+  </si>
+  <si>
+    <t>@BMT,</t>
+  </si>
+  <si>
+    <t>@UPDRS_I,</t>
+  </si>
+  <si>
+    <t>@UPDRS_II,</t>
+  </si>
+  <si>
+    <t>@UPDRS_18,</t>
+  </si>
+  <si>
+    <t>@UPDRS_19 ,</t>
+  </si>
+  <si>
+    <t>@UPDRS_20_FaceLipsChin,</t>
+  </si>
+  <si>
+    <t>@UPDRS_20_RHand,</t>
+  </si>
+  <si>
+    <t>@UPDRS_20_LHand,</t>
+  </si>
+  <si>
+    <t>@UPDRS_20_RFoot,</t>
+  </si>
+  <si>
+    <t>@UPDRS_20_LFoot,</t>
+  </si>
+  <si>
+    <t>@UPDRS_21_RHand,</t>
+  </si>
+  <si>
+    <t>@UPDRS_21_LHand,</t>
+  </si>
+  <si>
+    <t>@UPDRS_22_Neck,</t>
+  </si>
+  <si>
+    <t>@UPDRS_22_RHand,</t>
+  </si>
+  <si>
+    <t>@UPDRS_22_LHand,</t>
+  </si>
+  <si>
+    <t>@UPDRS_22_RFoot,</t>
+  </si>
+  <si>
+    <t>@UPDRS_22_LFoot,</t>
+  </si>
+  <si>
+    <t>@UPDRS_23_R,</t>
+  </si>
+  <si>
+    <t>@UPDRS_23_L,</t>
+  </si>
+  <si>
+    <t>@UPDRS_24_R,</t>
+  </si>
+  <si>
+    <t>@UPDRS_24_L,</t>
+  </si>
+  <si>
+    <t>@UPDRS_25_R,</t>
+  </si>
+  <si>
+    <t>@UPDRS_25_L,</t>
+  </si>
+  <si>
+    <t>@UPDRS_26_R,</t>
+  </si>
+  <si>
+    <t>@UPDRS_26_L,</t>
+  </si>
+  <si>
+    <t>@UPDRS_27,</t>
+  </si>
+  <si>
+    <t>@UPDRS_28,</t>
+  </si>
+  <si>
+    <t>@UPDRS_29,</t>
+  </si>
+  <si>
+    <t>@UPDRS_30,</t>
+  </si>
+  <si>
+    <t>@UPDRS_31,</t>
+  </si>
+  <si>
+    <t>@UPDRS_III,</t>
+  </si>
+  <si>
+    <t>@UPDRS_IV,</t>
+  </si>
+  <si>
+    <t>@UPDRS_TOTAL,</t>
+  </si>
+  <si>
+    <t>@HYscale,</t>
+  </si>
+  <si>
+    <t>@SchwabEnglandScale,</t>
+  </si>
+  <si>
+    <t>@OkulografiaUrzadzenie,</t>
+  </si>
+  <si>
+    <t>@Wideo</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>dopuszczalne wartości: 0, 1, 1.5, 2, 2.5, 3, 4, 5</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1365,6 +1485,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -1737,8 +1858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1874,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1773,7 +1894,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B3" s="43" t="s">
         <v>4</v>
@@ -1818,21 +1939,21 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="57" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" s="44" t="s">
         <v>231</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>232</v>
-      </c>
       <c r="D7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="57" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C8" s="44" t="s">
         <v>9</v>
@@ -1855,10 +1976,10 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>10</v>
@@ -1870,10 +1991,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1881,17 +2002,17 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>240</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>241</v>
       </c>
       <c r="D12" s="31"/>
       <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B13" s="76" t="s">
         <v>19</v>
@@ -1903,7 +2024,7 @@
         <v>20</v>
       </c>
       <c r="E13" s="67" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1927,7 +2048,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -2068,7 +2189,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>106</v>
@@ -2267,7 +2388,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>221</v>
@@ -2425,7 +2546,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>56</v>
@@ -2487,13 +2608,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D65" s="60" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E65" s="4"/>
     </row>
@@ -2522,7 +2643,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>78</v>
@@ -2850,10 +2971,10 @@
     </row>
     <row r="95" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>229</v>
+        <v>273</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>9</v>
@@ -2867,14 +2988,14 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B96" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C96" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D96" s="17"/>
       <c r="E96" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
@@ -3199,23 +3320,25 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B129" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C129" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D129" s="21"/>
+      <c r="D129" s="21" t="s">
+        <v>313</v>
+      </c>
       <c r="E129" s="21"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B130" s="56" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C130" s="33" t="s">
         <v>9</v>
       </c>
       <c r="D130" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E130" s="20"/>
     </row>
@@ -3230,7 +3353,7 @@
         <v>227</v>
       </c>
       <c r="E131" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -3246,7 +3369,7 @@
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B133" s="54" t="s">
         <v>173</v>
@@ -3341,7 +3464,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B142" s="39" t="s">
         <v>181</v>
@@ -3428,7 +3551,7 @@
     </row>
     <row r="149" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>156</v>
@@ -3472,19 +3595,19 @@
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="50"/>
       <c r="B153" s="63" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C153" s="64" t="s">
         <v>182</v>
       </c>
       <c r="D153" s="64"/>
       <c r="E153" s="64" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>160</v>
@@ -3511,7 +3634,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>9</v>
@@ -3521,7 +3644,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>9</v>
@@ -3622,17 +3745,17 @@
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="50"/>
       <c r="B167" s="68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C167" s="64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D167" s="64"/>
       <c r="E167" s="69"/>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B168" s="4" t="s">
         <v>193</v>
@@ -3703,16 +3826,16 @@
         <v>9</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E174" s="2"/>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B175" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="C175" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
@@ -3863,15 +3986,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:FW31"/>
+  <dimension ref="B3:FW95"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:M16"/>
+    <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.42578125" style="70"/>
+    <col min="1" max="8" width="9.42578125" style="70"/>
+    <col min="9" max="9" width="29.140625" style="70" customWidth="1"/>
     <col min="10" max="10" width="50.140625" style="70" customWidth="1"/>
     <col min="11" max="11" width="65" style="70" customWidth="1"/>
     <col min="12" max="16384" width="9.42578125" style="70"/>
@@ -4250,13 +4374,13 @@
         <v>193</v>
       </c>
       <c r="K5" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>193</v>
       </c>
       <c r="M5" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N5" s="71"/>
       <c r="O5" s="71"/>
@@ -4438,13 +4562,13 @@
         <v>194</v>
       </c>
       <c r="K6" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>194</v>
       </c>
       <c r="M6" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N6" s="71"/>
       <c r="O6" s="71"/>
@@ -4626,13 +4750,13 @@
         <v>195</v>
       </c>
       <c r="K7" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>195</v>
       </c>
       <c r="M7" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N7" s="71"/>
       <c r="O7" s="71"/>
@@ -4814,13 +4938,13 @@
         <v>196</v>
       </c>
       <c r="K8" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>196</v>
       </c>
       <c r="M8" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N8" s="71"/>
       <c r="O8" s="71"/>
@@ -5002,13 +5126,13 @@
         <v>197</v>
       </c>
       <c r="K9" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>197</v>
       </c>
       <c r="M9" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N9" s="71"/>
       <c r="O9" s="71"/>
@@ -5190,13 +5314,13 @@
         <v>198</v>
       </c>
       <c r="K10" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>198</v>
       </c>
       <c r="M10" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N10" s="71"/>
       <c r="O10" s="71"/>
@@ -5378,13 +5502,13 @@
         <v>200</v>
       </c>
       <c r="K11" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>200</v>
       </c>
       <c r="M11" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N11" s="71"/>
       <c r="O11" s="71"/>
@@ -5563,16 +5687,16 @@
       <c r="H12" s="71"/>
       <c r="I12" s="73"/>
       <c r="J12" s="30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K12" s="71" t="s">
+        <v>268</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="M12" s="71" t="s">
         <v>269</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>237</v>
-      </c>
-      <c r="M12" s="71" t="s">
-        <v>270</v>
       </c>
       <c r="N12" s="71"/>
       <c r="O12" s="71"/>
@@ -5754,13 +5878,13 @@
         <v>201</v>
       </c>
       <c r="K13" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>201</v>
       </c>
       <c r="M13" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N13" s="71"/>
       <c r="O13" s="71"/>
@@ -5942,13 +6066,13 @@
         <v>202</v>
       </c>
       <c r="K14" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>202</v>
       </c>
       <c r="M14" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N14" s="71"/>
       <c r="O14" s="71"/>
@@ -6130,13 +6254,13 @@
         <v>203</v>
       </c>
       <c r="K15" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>203</v>
       </c>
       <c r="M15" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N15" s="71"/>
       <c r="O15" s="71"/>
@@ -6318,13 +6442,13 @@
         <v>204</v>
       </c>
       <c r="K16" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L16" s="42" t="s">
         <v>204</v>
       </c>
       <c r="M16" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N16" s="71"/>
       <c r="O16" s="71"/>
@@ -6504,11 +6628,11 @@
       <c r="I17" s="73"/>
       <c r="J17" s="31"/>
       <c r="K17" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L17" s="31"/>
       <c r="M17" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N17" s="71"/>
       <c r="O17" s="71"/>
@@ -6688,11 +6812,11 @@
       <c r="I18" s="73"/>
       <c r="J18" s="68"/>
       <c r="K18" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L18" s="68"/>
       <c r="M18" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N18" s="71"/>
       <c r="O18" s="71"/>
@@ -6872,11 +6996,11 @@
       <c r="I19" s="73"/>
       <c r="J19" s="78"/>
       <c r="K19" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L19" s="78"/>
       <c r="M19" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N19" s="71"/>
       <c r="O19" s="71"/>
@@ -7056,11 +7180,11 @@
       <c r="I20" s="73"/>
       <c r="J20" s="78"/>
       <c r="K20" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L20" s="78"/>
       <c r="M20" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N20" s="71"/>
       <c r="O20" s="71"/>
@@ -7240,11 +7364,11 @@
       <c r="I21" s="73"/>
       <c r="J21" s="78"/>
       <c r="K21" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L21" s="78"/>
       <c r="M21" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N21" s="71"/>
       <c r="O21" s="71"/>
@@ -7424,11 +7548,11 @@
       <c r="I22" s="73"/>
       <c r="J22" s="78"/>
       <c r="K22" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L22" s="78"/>
       <c r="M22" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N22" s="71"/>
       <c r="O22" s="71"/>
@@ -7608,11 +7732,11 @@
       <c r="I23" s="73"/>
       <c r="J23" s="78"/>
       <c r="K23" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L23" s="78"/>
       <c r="M23" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N23" s="71"/>
       <c r="O23" s="71"/>
@@ -7792,11 +7916,11 @@
       <c r="I24" s="73"/>
       <c r="J24" s="78"/>
       <c r="K24" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L24" s="78"/>
       <c r="M24" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N24" s="71"/>
       <c r="O24" s="71"/>
@@ -7976,11 +8100,11 @@
       <c r="I25" s="73"/>
       <c r="J25" s="78"/>
       <c r="K25" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L25" s="78"/>
       <c r="M25" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N25" s="71"/>
       <c r="O25" s="71"/>
@@ -8160,11 +8284,11 @@
       <c r="I26" s="73"/>
       <c r="J26" s="78"/>
       <c r="K26" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L26" s="78"/>
       <c r="M26" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N26" s="71"/>
       <c r="O26" s="71"/>
@@ -8344,11 +8468,11 @@
       <c r="I27" s="73"/>
       <c r="J27" s="78"/>
       <c r="K27" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L27" s="78"/>
       <c r="M27" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N27" s="71"/>
       <c r="O27" s="71"/>
@@ -8528,11 +8652,11 @@
       <c r="I28" s="73"/>
       <c r="J28" s="78"/>
       <c r="K28" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L28" s="78"/>
       <c r="M28" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N28" s="71"/>
       <c r="O28" s="71"/>
@@ -8708,11 +8832,11 @@
       <c r="G29" s="71"/>
       <c r="J29" s="78"/>
       <c r="K29" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L29" s="78"/>
       <c r="M29" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="2:179" x14ac:dyDescent="0.25">
@@ -8722,11 +8846,11 @@
       <c r="G30" s="71"/>
       <c r="J30" s="78"/>
       <c r="K30" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L30" s="78"/>
       <c r="M30" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="2:179" x14ac:dyDescent="0.25">
@@ -8736,11 +8860,634 @@
       <c r="G31" s="71"/>
       <c r="J31" s="78"/>
       <c r="K31" s="71" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L31" s="78"/>
       <c r="M31" s="71" t="s">
-        <v>270</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I35" s="70" t="s">
+        <v>273</v>
+      </c>
+      <c r="J35" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K35" s="70" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I36" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="J36" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K36" s="70" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="70" t="s">
+        <v>124</v>
+      </c>
+      <c r="J37" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K37" s="70" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I38" s="70" t="s">
+        <v>125</v>
+      </c>
+      <c r="J38" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K38" s="70" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I39" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="J39" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K39" s="70" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I40" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="J40" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K40" s="70" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I41" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="J41" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K41" s="70" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="I42" s="70" t="s">
+        <v>132</v>
+      </c>
+      <c r="J42" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K42" s="70" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D43" s="70">
+        <v>0</v>
+      </c>
+      <c r="I43" s="70" t="s">
+        <v>133</v>
+      </c>
+      <c r="J43" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K43" s="70" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D44" s="70">
+        <v>1</v>
+      </c>
+      <c r="I44" s="70" t="s">
+        <v>134</v>
+      </c>
+      <c r="J44" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K44" s="70" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D45" s="70">
+        <v>2</v>
+      </c>
+      <c r="I45" s="70" t="s">
+        <v>135</v>
+      </c>
+      <c r="J45" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K45" s="70" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D46" s="70">
+        <v>3</v>
+      </c>
+      <c r="I46" s="70" t="s">
+        <v>136</v>
+      </c>
+      <c r="J46" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K46" s="70" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D47" s="70">
+        <v>4</v>
+      </c>
+      <c r="I47" s="70" t="s">
+        <v>137</v>
+      </c>
+      <c r="J47" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K47" s="70" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D48" s="70">
+        <v>5</v>
+      </c>
+      <c r="I48" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="J48" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K48" s="70" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D49" s="70">
+        <v>6</v>
+      </c>
+      <c r="I49" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="J49" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K49" s="70" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D50" s="70">
+        <v>7</v>
+      </c>
+      <c r="I50" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="J50" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K50" s="70" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D51" s="70">
+        <v>8</v>
+      </c>
+      <c r="I51" s="70" t="s">
+        <v>141</v>
+      </c>
+      <c r="J51" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K51" s="70" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D52" s="70">
+        <v>9</v>
+      </c>
+      <c r="I52" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="J52" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K52" s="70" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D53" s="70">
+        <v>10</v>
+      </c>
+      <c r="I53" s="70" t="s">
+        <v>143</v>
+      </c>
+      <c r="J53" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K53" s="70" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D54" s="70">
+        <v>11</v>
+      </c>
+      <c r="I54" s="70" t="s">
+        <v>144</v>
+      </c>
+      <c r="J54" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K54" s="70" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D55" s="70">
+        <v>12</v>
+      </c>
+      <c r="I55" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="J55" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K55" s="70" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D56" s="70">
+        <v>13</v>
+      </c>
+      <c r="I56" s="70" t="s">
+        <v>146</v>
+      </c>
+      <c r="J56" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K56" s="70" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D57" s="70">
+        <v>14</v>
+      </c>
+      <c r="I57" s="70" t="s">
+        <v>147</v>
+      </c>
+      <c r="J57" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K57" s="70" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D58" s="70">
+        <v>15</v>
+      </c>
+      <c r="I58" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="J58" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K58" s="70" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D59" s="70">
+        <v>16</v>
+      </c>
+      <c r="I59" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="J59" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K59" s="70" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D60" s="70">
+        <v>17</v>
+      </c>
+      <c r="I60" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="J60" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K60" s="70" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D61" s="70">
+        <v>18</v>
+      </c>
+      <c r="I61" s="70" t="s">
+        <v>151</v>
+      </c>
+      <c r="J61" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K61" s="70" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="62" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D62" s="70">
+        <v>19</v>
+      </c>
+      <c r="I62" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="J62" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K62" s="70" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D63" s="70">
+        <v>20</v>
+      </c>
+      <c r="I63" s="70" t="s">
+        <v>153</v>
+      </c>
+      <c r="J63" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K63" s="70" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D64" s="70">
+        <v>21</v>
+      </c>
+      <c r="I64" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="J64" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K64" s="70" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65" s="70">
+        <v>22</v>
+      </c>
+      <c r="I65" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="J65" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K65" s="70" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D66" s="70">
+        <v>23</v>
+      </c>
+      <c r="I66" s="70" t="s">
+        <v>126</v>
+      </c>
+      <c r="J66" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K66" s="70" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D67" s="70">
+        <v>24</v>
+      </c>
+      <c r="I67" s="70" t="s">
+        <v>127</v>
+      </c>
+      <c r="J67" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K67" s="70" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D68" s="70">
+        <v>25</v>
+      </c>
+      <c r="I68" s="70" t="s">
+        <v>128</v>
+      </c>
+      <c r="J68" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K68" s="70" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D69" s="70">
+        <v>26</v>
+      </c>
+      <c r="I69" s="70" t="s">
+        <v>242</v>
+      </c>
+      <c r="J69" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K69" s="70" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D70" s="70">
+        <v>27</v>
+      </c>
+      <c r="I70" s="70" t="s">
+        <v>243</v>
+      </c>
+      <c r="J70" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K70" s="70" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D71" s="70">
+        <v>28</v>
+      </c>
+      <c r="I71" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="J71" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K71" s="70" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D72" s="70">
+        <v>29</v>
+      </c>
+      <c r="I72" s="70" t="s">
+        <v>225</v>
+      </c>
+      <c r="J72" s="79" t="s">
+        <v>312</v>
+      </c>
+      <c r="K72" s="70" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D73" s="70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D74" s="70">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D75" s="70">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D76" s="70">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="77" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D77" s="70">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D78" s="70">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D79" s="70">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D80" s="70">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="70">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="70">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="70">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="70">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="70">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="70">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D87" s="70">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D88" s="70">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D89" s="70">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D90" s="70">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D91" s="70">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D92" s="70">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D93" s="70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D94" s="70">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D95" s="70">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>